<commit_message>
updated with new cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F651B187-DCBA-49A8-BB4B-E8542E41CC79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7212A37-5921-4A51-9418-5AAFE4B7DDE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="222">
   <si>
     <t>TSID</t>
   </si>
@@ -760,19 +760,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Fail:getTextGuidedTipsToastMessage is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //span[contains(.,'You are in Help mode. Use the toggle in the Support menu to turn the tips on and off any time.')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@544b805b (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.61.204', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 90.0.4430.212, chrome: {chromedriverVersion: 90.0.4430.24 (4c6d850f087da..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56363}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 00d4d616dde44e10f0dc66aae735c442getTextGuidedTipsToastMessage is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //span[contains(.,'You are in Help mode. Use the toggle in the Support menu to turn the tips on and off any time.')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@544b805b (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.61.204', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 90.0.4430.212, chrome: {chromedriverVersion: 90.0.4430.24 (4c6d850f087da..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56363}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 00d4d616dde44e10f0dc66aae735c442</t>
   </si>
 </sst>
 </file>
@@ -1337,9 +1324,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="25.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="35.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1374,24 +1361,24 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="65.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="45.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="9.765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="255.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="37.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="70.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="40.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="14.7109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
-    <col min="13" max="16384" style="4" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="255" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="70.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="40" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="8.85546875" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2130,7 +2117,7 @@
         <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
Changed Password of credentials
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F651B187-DCBA-49A8-BB4B-E8542E41CC79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63F97D1-FDB9-421B-8F6E-53395FCB12D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="248">
   <si>
     <t>TSID</t>
   </si>
@@ -686,9 +686,6 @@
     <t>rashmi.rl@thomsonreuters.com</t>
   </si>
   <si>
-    <t>Admin@123</t>
-  </si>
-  <si>
     <t>CheckboxSelection</t>
   </si>
   <si>
@@ -746,33 +743,239 @@
     <t>ES198601278A</t>
   </si>
   <si>
-    <t>Fail: java.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //body[contains(text(),'PDF is not available')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@125855a3 (tried for 50 second(s) with 500 milliseconds interval)
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>smiles</t>
+  </si>
+  <si>
+    <t>Fail:waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2e32a8c4 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.61.204', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 90.0.4430.212, chrome: {chromedriverVersion: 90.0.4430.24 (4c6d850f087da..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63370}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 7c5aecfb86feda4f648a56f8f452bf6a java.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //body[contains(text(),'PDF is not available')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@125855a3 (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61426}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 53ad33f3cc438da53e2c48224f39c0fcwaitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2e32a8c4 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.61.204', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 90.0.4430.212, chrome: {chromedriverVersion: 90.0.4430.24 (4c6d850f087da..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63370}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 7c5aecfb86feda4f648a56f8f452bf6a</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Fail:getTextGuidedTipsToastMessage is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //span[contains(.,'You are in Help mode. Use the toggle in the Support menu to turn the tips on and off any time.')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@544b805b (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61426}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 53ad33f3cc438da53e2c48224f39c0fc</t>
+  </si>
+  <si>
+    <t>Rerun</t>
+  </si>
+  <si>
+    <t>Fail:click on Button Tab Insights is not working for :: java.lang.NullPointerExceptionclick on Button Tab Insights is not working for :: java.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>Fail:clickOnThumbsUpIcon is not workingjava.lang.NullPointerExceptionclickOnThumbsUpIcon is not workingjava.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>Fail:Title Field is not displayed for given row in Literature results page.Title is not displayed for given row in Patent results page.Patent tab is not displayed in results page.Literature tab is not displayed in results page.SearchBox is not displayed next to Liturature Tab.</t>
+  </si>
+  <si>
+    <t>Fail:nullnull</t>
+  </si>
+  <si>
+    <t>Fail:hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@37489e45 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.61.204', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 90.0.4430.212, chrome: {chromedriverVersion: 90.0.4430.24 (4c6d850f087da..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56363}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 00d4d616dde44e10f0dc66aae735c442getTextGuidedTipsToastMessage is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //span[contains(.,'You are in Help mode. Use the toggle in the Support menu to turn the tips on and off any time.')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@544b805b (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60833}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 86aaf565f74f4903c6a42e2001cd98d1hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@37489e45 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.61.204', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 90.0.4430.212, chrome: {chromedriverVersion: 90.0.4430.24 (4c6d850f087da..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56363}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 00d4d616dde44e10f0dc66aae735c442</t>
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60833}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 86aaf565f74f4903c6a42e2001cd98d1</t>
+  </si>
+  <si>
+    <t>Fail:hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@206d7f15 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55555}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 8adf3a36bb0fca3958115472e66174e6hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@206d7f15 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55555}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 8adf3a36bb0fca3958115472e66174e6</t>
+  </si>
+  <si>
+    <t>Fail:Toast Message has not been displayed.Search box accepted morethan 2000 characters</t>
+  </si>
+  <si>
+    <t>Fail:getColorOfPillBox is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]"}
+  (Session info: chrome=91.0.4472.124)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51235}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: d2275a66ca0ccabe24b119ce462f12d1
+*** Element info: {Using=xpath, value=(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]}getColorOfPillBox is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]"}
+  (Session info: chrome=91.0.4472.124)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51235}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: d2275a66ca0ccabe24b119ce462f12d1
+*** Element info: {Using=xpath, value=(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]}</t>
+  </si>
+  <si>
+    <t>Fail:isDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerExceptionisDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>Fail:ClearAll button is in disable modeclickOnbutton ClearAll Filters is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//span[@class='mat-button-wrapper'][contains(.,'Clear all')]"}
+  (Session info: chrome=91.0.4472.124)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58036}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 5e99098926a26aab6a7e744f4ebe47d9
+*** Element info: {Using=xpath, value=//span[@class='mat-button-wrapper'][contains(.,'Clear all')]}clickOnbutton ClearAll Filters is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//span[@class='mat-button-wrapper'][contains(.,'Clear all')]"}
+  (Session info: chrome=91.0.4472.124)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58036}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 5e99098926a26aab6a7e744f4ebe47d9
+*** Element info: {Using=xpath, value=//span[@class='mat-button-wrapper'][contains(.,'Clear all')]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail:clickOnExpandDropdown is not working waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: (//section[@class='filter-details']//div[@class='mat-form-field-infix']//mat-icon)[1]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@cf08bec (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61364}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a9c619a601bbd29729595f9063780838clickOnExpandDropdown is not working waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: (//section[@class='filter-details']//div[@class='mat-form-field-infix']//mat-icon)[1]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@cf08bec (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61364}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a9c619a601bbd29729595f9063780838Results are not get refreshed </t>
+  </si>
+  <si>
+    <t>Fail:PDF window opens has not opened</t>
+  </si>
+  <si>
+    <t>Fail:dropdown value has not fetchedjava.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@class='mat-select-value']/span/span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@615e555d (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60020}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 9c29b511e0f7295e7accff85995be0d8dropdown value has not fetchedjava.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@class='mat-select-value']/span/span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@615e555d (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60020}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 9c29b511e0f7295e7accff85995be0d8</t>
+  </si>
+  <si>
+    <t>Fail:RESULT SETS ARE NOT REFRESHED  : 	0		 :	1759456RESULT SETS ARE NOT REFRESHED : 	0		 AFTER FILTER :	1759456</t>
+  </si>
+  <si>
+    <t>Fail:INVENTOR FILTER FIELD  IS ENABLED</t>
+  </si>
+  <si>
+    <t>Fail:Inventor filter field  IS ENABLED</t>
+  </si>
+  <si>
+    <t>Fail:checkbox is not selectedjava.lang.Exception: jsClick is not  working on:: [[ChromeDriver: chrome on WINDOWS (9ef33598e97cc300166e18f03587e4d5)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on WINDOWS (9ef33598e97cc300166e18f03587e4d5)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57543}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 9ef33598e97cc300166e18f03587e4d5checkbox is not selectedjava.lang.Exception: jsClick is not  working on:: [[ChromeDriver: chrome on WINDOWS (9ef33598e97cc300166e18f03587e4d5)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on WINDOWS (9ef33598e97cc300166e18f03587e4d5)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57543}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 9ef33598e97cc300166e18f03587e4d5</t>
+  </si>
+  <si>
+    <t>Fail:checkbox is not selectedjava.lang.Exception: jsClick is not  working on:: [[ChromeDriver: chrome on WINDOWS (ac4881dbb7541956be0c94efa15cb71a)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on WINDOWS (ac4881dbb7541956be0c94efa15cb71a)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55134}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: ac4881dbb7541956be0c94efa15cb71acheckbox is not selectedjava.lang.Exception: jsClick is not  working on:: [[ChromeDriver: chrome on WINDOWS (ac4881dbb7541956be0c94efa15cb71a)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on WINDOWS (ac4881dbb7541956be0c94efa15cb71a)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55134}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: ac4881dbb7541956be0c94efa15cb71a</t>
+  </si>
+  <si>
+    <t>Fail:RESULT SETS ARE NOT REFRESHED  : 	28551		 AFTER FILTER :	154waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; aside &gt; div:nth-child(1) &gt; span.pn' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@27de4165 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63655}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: b7c44885cd7be62fb773220e779c505bwaitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; aside &gt; div:nth-child(1) &gt; span.pn' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@27de4165 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63655}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: b7c44885cd7be62fb773220e779c505b</t>
+  </si>
+  <si>
+    <t>Fail:getTextLiteratureTitle is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"css selector","selector":"app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-header &gt; div &gt; mat-card-subtitle"}
+  (Session info: chrome=91.0.4472.124)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56914}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: c9f312d12df25e39d309a236c704c38d
+*** Element info: {Using=css selector, value=app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-header &gt; div &gt; mat-card-subtitle}getTextLiteratureTitle is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"css selector","selector":"app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-header &gt; div &gt; mat-card-subtitle"}
+  (Session info: chrome=91.0.4472.124)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56914}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: c9f312d12df25e39d309a236c704c38d
+*** Element info: {Using=css selector, value=app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-header &gt; div &gt; mat-card-subtitle}</t>
+  </si>
+  <si>
+    <t>Fail:clickOnMoreFiltersDropdown is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@class='mat-select-arrow']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@40a1ff79 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60427}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 2cc58071c0117c7a31960630ab7b60e9clickOnMoreFiltersDropdown is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@class='mat-select-arrow']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@40a1ff79 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60427}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 2cc58071c0117c7a31960630ab7b60e9</t>
+  </si>
+  <si>
+    <t>Fail:clickOnLinkCitingPatent is not workingjava.lang.Exception: jsClick is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: (//mat-panel-title[contains(@class,'mat-expansion-panel-header-title citation-headers')])[1]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: (//mat-panel-title[contains(@class,'mat-expansion-panel-header-title citation-headers')])[1]' (tried for 50 second(s) with 500 milliseconds interval)clickOnLinkCitingPatent is not workingjava.lang.Exception: jsClick is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: (//mat-panel-title[contains(@class,'mat-expansion-panel-header-title citation-headers')])[1]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: (//mat-panel-title[contains(@class,'mat-expansion-panel-header-title citation-headers')])[1]' (tried for 50 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>Fail:setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-placeholder='Type folder name']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-placeholder='Type folder name']' (tried for 50 second(s) with 500 milliseconds interval)setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-placeholder='Type folder name']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-placeholder='Type folder name']' (tried for 50 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>Fail:clickOnCitingPatentViewASResultSet is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (26a2606bc0f59e6c132214108e51d4a9)] -&gt; xpath: (//span[contains(.,'View as result set')])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@34fa4ff7 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50777}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 26a2606bc0f59e6c132214108e51d4a9clickOnCitingPatentViewASResultSet is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (26a2606bc0f59e6c132214108e51d4a9)] -&gt; xpath: (//span[contains(.,'View as result set')])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@34fa4ff7 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50777}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 26a2606bc0f59e6c132214108e51d4a9</t>
+  </si>
+  <si>
+    <t>Fail:setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' (tried for 50 second(s) with 500 milliseconds interval)setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' (tried for 50 second(s) with 500 milliseconds interval)</t>
   </si>
 </sst>
 </file>
@@ -1337,9 +1540,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="25.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="35.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1371,30 +1574,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="65.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="45.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="9.765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="255.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="37.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="70.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="40.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="14.7109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
-    <col min="13" max="16384" style="4" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="59" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="255" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="70.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="40" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="8.85546875" style="4" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1434,8 +1637,11 @@
       <c r="M1" s="4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>82</v>
       </c>
@@ -1449,22 +1655,22 @@
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" t="s">
         <v>221</v>
       </c>
-      <c r="F2" t="s">
-        <v>176</v>
-      </c>
       <c r="G2" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>83</v>
       </c>
@@ -1478,22 +1684,22 @@
         <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>176</v>
+        <v>223</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>84</v>
       </c>
@@ -1507,22 +1713,22 @@
         <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F4" t="s">
-        <v>176</v>
+        <v>224</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>85</v>
       </c>
@@ -1536,22 +1742,22 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F5" t="s">
-        <v>176</v>
+        <v>225</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>206</v>
-      </c>
       <c r="I5" s="20" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -1565,22 +1771,22 @@
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F6" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>87</v>
       </c>
@@ -1594,16 +1800,16 @@
         <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
         <v>176</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>31</v>
@@ -1612,7 +1818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>88</v>
       </c>
@@ -1626,16 +1832,16 @@
         <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>176</v>
+        <v>227</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>35</v>
@@ -1644,7 +1850,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>89</v>
       </c>
@@ -1658,16 +1864,16 @@
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F9" t="s">
-        <v>176</v>
+        <v>228</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>35</v>
@@ -1676,7 +1882,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>90</v>
       </c>
@@ -1690,22 +1896,22 @@
         <v>40</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F10" t="s">
-        <v>176</v>
+        <v>229</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>91</v>
       </c>
@@ -1719,16 +1925,16 @@
         <v>43</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F11" t="s">
-        <v>176</v>
+        <v>230</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>20</v>
@@ -1737,7 +1943,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>92</v>
       </c>
@@ -1751,16 +1957,16 @@
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F12" t="s">
         <v>176</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>20</v>
@@ -1769,7 +1975,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>94</v>
       </c>
@@ -1783,16 +1989,16 @@
         <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F13" t="s">
-        <v>176</v>
+        <v>231</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>20</v>
@@ -1801,7 +2007,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>95</v>
       </c>
@@ -1815,16 +2021,16 @@
         <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F14" t="s">
-        <v>176</v>
+        <v>231</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>20</v>
@@ -1833,7 +2039,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>96</v>
       </c>
@@ -1847,16 +2053,16 @@
         <v>52</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F15" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>35</v>
@@ -1865,7 +2071,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>97</v>
       </c>
@@ -1879,19 +2085,19 @@
         <v>61</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>206</v>
-      </c>
       <c r="I16" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K16" s="2"/>
     </row>
@@ -1909,16 +2115,16 @@
         <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>176</v>
+        <v>232</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>17</v>
@@ -1940,7 +2146,7 @@
         <v>67</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>176</v>
@@ -1949,7 +2155,7 @@
         <v>199</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>68</v>
@@ -1970,16 +2176,16 @@
         <v>64</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>176</v>
+        <v>233</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>17</v>
@@ -2001,7 +2207,7 @@
         <v>77</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>176</v>
@@ -2010,7 +2216,7 @@
         <v>199</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>23</v>
@@ -2032,7 +2238,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>176</v>
@@ -2041,7 +2247,7 @@
         <v>199</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>103</v>
@@ -2059,7 +2265,7 @@
         <v>105</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>14</v>
@@ -2068,16 +2274,16 @@
         <v>75</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>176</v>
+        <v>234</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>106</v>
@@ -2099,16 +2305,16 @@
         <v>56</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="H23" s="19" t="s">
-        <v>200</v>
+      <c r="H23" s="18" t="s">
+        <v>219</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>23</v>
@@ -2130,7 +2336,7 @@
         <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>176</v>
@@ -2139,7 +2345,7 @@
         <v>199</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
@@ -2158,7 +2364,7 @@
         <v>60</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>176</v>
@@ -2167,7 +2373,7 @@
         <v>199</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>23</v>
@@ -2189,7 +2395,7 @@
         <v>79</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>176</v>
@@ -2198,7 +2404,7 @@
         <v>199</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>103</v>
@@ -2220,7 +2426,7 @@
         <v>72</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>176</v>
@@ -2229,7 +2435,7 @@
         <v>199</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>73</v>
@@ -2253,16 +2459,16 @@
         <v>112</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>176</v>
+        <v>236</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>115</v>
@@ -2282,7 +2488,7 @@
         <v>118</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>176</v>
@@ -2291,7 +2497,7 @@
         <v>199</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>106</v>
@@ -2311,7 +2517,7 @@
         <v>121</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>176</v>
@@ -2320,7 +2526,7 @@
         <v>199</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>106</v>
@@ -2340,16 +2546,16 @@
         <v>124</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>176</v>
+        <v>237</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>106</v>
@@ -2369,16 +2575,16 @@
         <v>126</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>176</v>
+        <v>238</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>106</v>
@@ -2398,7 +2604,7 @@
         <v>129</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>176</v>
@@ -2407,7 +2613,7 @@
         <v>199</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>106</v>
@@ -2427,7 +2633,7 @@
         <v>132</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>176</v>
@@ -2436,7 +2642,7 @@
         <v>199</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>106</v>
@@ -2456,7 +2662,7 @@
         <v>134</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>176</v>
@@ -2465,7 +2671,7 @@
         <v>199</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>106</v>
@@ -2485,7 +2691,7 @@
         <v>136</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>176</v>
@@ -2494,7 +2700,7 @@
         <v>199</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>106</v>
@@ -2515,7 +2721,7 @@
         <v>139</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F37" s="13" t="s">
         <v>176</v>
@@ -2524,7 +2730,7 @@
         <v>199</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I37" s="12" t="s">
         <v>115</v>
@@ -2545,7 +2751,7 @@
         <v>142</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F38" s="13" t="s">
         <v>176</v>
@@ -2554,7 +2760,7 @@
         <v>199</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I38" s="12" t="s">
         <v>115</v>
@@ -2575,7 +2781,7 @@
         <v>145</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F39" s="13" t="s">
         <v>176</v>
@@ -2584,7 +2790,7 @@
         <v>199</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I39" s="12" t="s">
         <v>115</v>
@@ -2605,7 +2811,7 @@
         <v>148</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>176</v>
@@ -2614,7 +2820,7 @@
         <v>199</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I40" s="12" t="s">
         <v>115</v>
@@ -2635,7 +2841,7 @@
         <v>151</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>176</v>
@@ -2644,7 +2850,7 @@
         <v>199</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I41" s="12" t="s">
         <v>115</v>
@@ -2664,7 +2870,7 @@
         <v>154</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>176</v>
@@ -2673,7 +2879,7 @@
         <v>199</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I42" s="12" t="s">
         <v>115</v>
@@ -2699,10 +2905,10 @@
         <v>176</v>
       </c>
       <c r="G43" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H43" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="H43" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>157</v>
@@ -2722,16 +2928,16 @@
         <v>159</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F44" t="s">
-        <v>176</v>
+        <v>239</v>
       </c>
       <c r="G44" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H44" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="H44" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>20</v>
@@ -2751,16 +2957,16 @@
         <v>161</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F45" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="G45" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H45" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="H45" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>20</v>
@@ -2780,16 +2986,16 @@
         <v>162</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F46" t="s">
         <v>176</v>
       </c>
       <c r="G46" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H46" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>163</v>
@@ -2809,16 +3015,16 @@
         <v>164</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F47" t="s">
         <v>176</v>
       </c>
       <c r="G47" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H47" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>165</v>
@@ -2838,16 +3044,16 @@
         <v>166</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F48" t="s">
         <v>176</v>
       </c>
       <c r="G48" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H48" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="H48" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>23</v>
@@ -2867,16 +3073,16 @@
         <v>179</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F49" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="G49" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H49" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="H49" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>180</v>
@@ -2896,16 +3102,16 @@
         <v>182</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G50" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="H50" s="24" t="s">
         <v>205</v>
-      </c>
-      <c r="H50" s="24" t="s">
-        <v>206</v>
       </c>
       <c r="I50" s="22" t="s">
         <v>20</v>
@@ -2926,16 +3132,16 @@
         <v>184</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>176</v>
+        <v>243</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I51" s="12" t="s">
         <v>23</v>
@@ -2959,7 +3165,7 @@
         <v>187</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>176</v>
@@ -2968,7 +3174,7 @@
         <v>199</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I52" s="12" t="s">
         <v>103</v>
@@ -2988,16 +3194,16 @@
         <v>189</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="G53" s="18" t="s">
         <v>199</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>190</v>
@@ -3005,7 +3211,7 @@
     </row>
     <row r="54" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B54" s="22" t="s">
         <v>197</v>
@@ -3017,16 +3223,16 @@
         <v>198</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>176</v>
+        <v>245</v>
       </c>
       <c r="G54" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="H54" s="24" t="s">
-        <v>200</v>
+      <c r="H54" s="18" t="s">
+        <v>219</v>
       </c>
       <c r="I54" s="22" t="s">
         <v>103</v>
@@ -3035,19 +3241,19 @@
     </row>
     <row r="55" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B55" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>202</v>
-      </c>
       <c r="E55" s="4" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="F55" s="23" t="s">
         <v>176</v>
@@ -3055,8 +3261,8 @@
       <c r="G55" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="H55" s="24" t="s">
-        <v>200</v>
+      <c r="H55" s="18" t="s">
+        <v>219</v>
       </c>
       <c r="I55" s="22" t="s">
         <v>190</v>
@@ -3065,58 +3271,58 @@
     </row>
     <row r="56" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B56" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="C56" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="22" t="s">
+      <c r="E56" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="G56" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="F56" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="G56" s="22" t="s">
+      <c r="H56" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="H56" s="22" t="s">
-        <v>206</v>
-      </c>
       <c r="I56" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J56" s="25"/>
     </row>
     <row r="57" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B57" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="C57" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>208</v>
-      </c>
       <c r="E57" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F57" s="22" t="s">
-        <v>176</v>
+        <v>247</v>
       </c>
       <c r="G57" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H57" s="22" t="s">
         <v>205</v>
-      </c>
-      <c r="H57" s="22" t="s">
-        <v>206</v>
       </c>
       <c r="I57" s="22" t="s">
         <v>20</v>
@@ -3125,28 +3331,28 @@
     </row>
     <row r="58" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B58" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="C58" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>210</v>
-      </c>
       <c r="E58" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F58" s="22" t="s">
-        <v>176</v>
+        <v>247</v>
       </c>
       <c r="G58" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H58" s="22" t="s">
         <v>205</v>
-      </c>
-      <c r="H58" s="22" t="s">
-        <v>206</v>
       </c>
       <c r="I58" s="22" t="s">
         <v>23</v>
@@ -3160,54 +3366,41 @@
     <hyperlink ref="G17" r:id="rId1" xr:uid="{723970F4-4603-469C-B45C-96036D0B804A}"/>
     <hyperlink ref="H17" r:id="rId2" xr:uid="{2AD4D63B-2996-4EF0-8A2F-8AF5B6BD9CC8}"/>
     <hyperlink ref="G18:G33" r:id="rId3" display="rashmi.rl@thomsonreuters.com" xr:uid="{3DB5E2C0-A750-4358-9BF6-32D3D98D2096}"/>
-    <hyperlink ref="H18:H33" r:id="rId4" display="Admin@123" xr:uid="{BA92D6DD-AADB-4069-AFCB-839A6F14E232}"/>
-    <hyperlink ref="G33" r:id="rId5" xr:uid="{17A7C8C6-2597-4D73-A91A-12BAC045FE55}"/>
-    <hyperlink ref="G34" r:id="rId6" xr:uid="{5B70CB00-7AFC-441C-8B21-F20FFAC5C9AF}"/>
-    <hyperlink ref="G35" r:id="rId7" xr:uid="{52261ED4-7225-4B8F-970A-9E1807022FE1}"/>
-    <hyperlink ref="G36" r:id="rId8" xr:uid="{501C3C63-1543-43E6-8460-64278CEC18A9}"/>
-    <hyperlink ref="G37" r:id="rId9" xr:uid="{CDA235E6-241E-4DCC-ACAE-541EAE638029}"/>
-    <hyperlink ref="G38" r:id="rId10" xr:uid="{2CC833FE-2CFA-4F55-A03C-0F6D36B8FF1A}"/>
-    <hyperlink ref="G39" r:id="rId11" xr:uid="{7CB5209A-D384-479E-ABBE-818E4A32E00E}"/>
-    <hyperlink ref="H34" r:id="rId12" xr:uid="{844571CA-3BAD-467A-A34B-3A358EC13C1E}"/>
-    <hyperlink ref="H35" r:id="rId13" xr:uid="{68973837-B14A-4E03-86E4-985D4BC30277}"/>
-    <hyperlink ref="H36" r:id="rId14" xr:uid="{E5973375-6697-471D-BBCC-1169C0B3ED3D}"/>
-    <hyperlink ref="H37" r:id="rId15" xr:uid="{A778FDBC-52CD-41F2-ACD2-4FE7CE425AAD}"/>
-    <hyperlink ref="H38" r:id="rId16" xr:uid="{50A1E3B2-8159-4D87-A1FE-2D2F37C0272D}"/>
-    <hyperlink ref="H39" r:id="rId17" xr:uid="{B873B963-4DD0-4904-B0A5-116E0B3CD77A}"/>
-    <hyperlink ref="G40" r:id="rId18" xr:uid="{8398B387-7BC7-498B-9AA4-042A87D3A4DB}"/>
-    <hyperlink ref="H40" r:id="rId19" xr:uid="{048C8336-07F0-4FDE-8DB7-0B965C168F26}"/>
-    <hyperlink ref="G41" r:id="rId20" xr:uid="{F030BE8B-BC36-49E1-8D71-1478C5C4BCDF}"/>
-    <hyperlink ref="H41" r:id="rId21" xr:uid="{8B0D0D08-8A2C-4C34-BC5D-820B82A6579F}"/>
-    <hyperlink ref="G42" r:id="rId22" xr:uid="{23135E44-8E96-4D83-A082-A7511C1C0771}"/>
-    <hyperlink ref="H42" r:id="rId23" xr:uid="{335C4A8A-91EB-43FA-927A-A03E96ADF2D2}"/>
-    <hyperlink ref="G43" r:id="rId24" xr:uid="{0CCCEC04-DDD0-4D0F-8D23-C47F6F6CEC53}"/>
-    <hyperlink ref="H43" r:id="rId25" xr:uid="{D41C1E47-89D1-498E-802F-F4AA544A235B}"/>
-    <hyperlink ref="G44" r:id="rId26" xr:uid="{D466216C-1EF1-4553-A660-7BF606C27DB9}"/>
-    <hyperlink ref="G45" r:id="rId27" xr:uid="{F86289C3-3FA2-4BA4-AEDD-552CD06D34E6}"/>
-    <hyperlink ref="G46" r:id="rId28" xr:uid="{0DE6A34B-2C8E-4613-99BD-7169693A3191}"/>
-    <hyperlink ref="G47" r:id="rId29" xr:uid="{0E6F7DF1-DD17-41D2-B68A-807CE6F4A387}"/>
-    <hyperlink ref="G48" r:id="rId30" xr:uid="{111B4475-977A-49B9-9657-CCB615DEF79F}"/>
-    <hyperlink ref="G49" r:id="rId31" xr:uid="{471A5D33-835A-414E-97B8-362512B11F19}"/>
-    <hyperlink ref="G50" r:id="rId32" xr:uid="{C7E5B850-A6A3-47EB-B6C2-A656ABE578C3}"/>
-    <hyperlink ref="H44" r:id="rId33" xr:uid="{57BA88B1-4374-4605-B1CF-000FB7A9AD17}"/>
-    <hyperlink ref="H45" r:id="rId34" xr:uid="{1020C407-DE4D-45CD-B802-7B6DA3235B83}"/>
-    <hyperlink ref="H46" r:id="rId35" xr:uid="{4A959DA8-94AE-478F-AA59-3FF5B726B06D}"/>
-    <hyperlink ref="H47" r:id="rId36" xr:uid="{A2EA3677-590B-439E-B26B-BBB5D057F411}"/>
-    <hyperlink ref="H48" r:id="rId37" xr:uid="{E55440CE-A9F7-403D-B428-B5518F503072}"/>
-    <hyperlink ref="H49" r:id="rId38" xr:uid="{A922F6B7-45E9-4EC5-85E8-E946899CA468}"/>
-    <hyperlink ref="H50" r:id="rId39" xr:uid="{0AF8DC04-D1CF-4807-A710-B373CBBE5749}"/>
-    <hyperlink ref="G51" r:id="rId40" xr:uid="{4930390E-877B-48E6-806D-25B7F1D8C5B8}"/>
-    <hyperlink ref="H51" r:id="rId41" xr:uid="{8352E298-0BDE-450E-AE5B-924C8B5CB9CD}"/>
-    <hyperlink ref="G52" r:id="rId42" xr:uid="{F7B5D713-A9B5-4133-BD07-98197D7E72D4}"/>
-    <hyperlink ref="G53" r:id="rId43" xr:uid="{E5AB4738-A96D-4977-A386-A581CA3C01E6}"/>
-    <hyperlink ref="G54" r:id="rId44" xr:uid="{DE1E9284-2F49-42F1-A7C3-B0CEC31B6EFD}"/>
-    <hyperlink ref="G55" r:id="rId45" xr:uid="{E2B9685A-2447-4FE1-AF1B-C87EA1440D7B}"/>
-    <hyperlink ref="H52" r:id="rId46" xr:uid="{55C03EBD-3D41-4E5F-A435-4C0B2DEC9E55}"/>
-    <hyperlink ref="H53" r:id="rId47" xr:uid="{5341A66B-EA9D-4F56-9303-65E0631861C6}"/>
-    <hyperlink ref="H54" r:id="rId48" xr:uid="{C7DA9EE0-3D80-451F-9631-DF7414C08C9E}"/>
-    <hyperlink ref="H55" r:id="rId49" xr:uid="{47CAF88F-2E58-41EA-ABAE-C3F5EDFD7480}"/>
+    <hyperlink ref="G33" r:id="rId4" xr:uid="{17A7C8C6-2597-4D73-A91A-12BAC045FE55}"/>
+    <hyperlink ref="G34" r:id="rId5" xr:uid="{5B70CB00-7AFC-441C-8B21-F20FFAC5C9AF}"/>
+    <hyperlink ref="G35" r:id="rId6" xr:uid="{52261ED4-7225-4B8F-970A-9E1807022FE1}"/>
+    <hyperlink ref="G36" r:id="rId7" xr:uid="{501C3C63-1543-43E6-8460-64278CEC18A9}"/>
+    <hyperlink ref="G37" r:id="rId8" xr:uid="{CDA235E6-241E-4DCC-ACAE-541EAE638029}"/>
+    <hyperlink ref="G38" r:id="rId9" xr:uid="{2CC833FE-2CFA-4F55-A03C-0F6D36B8FF1A}"/>
+    <hyperlink ref="G39" r:id="rId10" xr:uid="{7CB5209A-D384-479E-ABBE-818E4A32E00E}"/>
+    <hyperlink ref="G40" r:id="rId11" xr:uid="{8398B387-7BC7-498B-9AA4-042A87D3A4DB}"/>
+    <hyperlink ref="G41" r:id="rId12" xr:uid="{F030BE8B-BC36-49E1-8D71-1478C5C4BCDF}"/>
+    <hyperlink ref="G42" r:id="rId13" xr:uid="{23135E44-8E96-4D83-A082-A7511C1C0771}"/>
+    <hyperlink ref="G43" r:id="rId14" xr:uid="{0CCCEC04-DDD0-4D0F-8D23-C47F6F6CEC53}"/>
+    <hyperlink ref="H43" r:id="rId15" xr:uid="{D41C1E47-89D1-498E-802F-F4AA544A235B}"/>
+    <hyperlink ref="G44" r:id="rId16" xr:uid="{D466216C-1EF1-4553-A660-7BF606C27DB9}"/>
+    <hyperlink ref="G45" r:id="rId17" xr:uid="{F86289C3-3FA2-4BA4-AEDD-552CD06D34E6}"/>
+    <hyperlink ref="G46" r:id="rId18" xr:uid="{0DE6A34B-2C8E-4613-99BD-7169693A3191}"/>
+    <hyperlink ref="G47" r:id="rId19" xr:uid="{0E6F7DF1-DD17-41D2-B68A-807CE6F4A387}"/>
+    <hyperlink ref="G48" r:id="rId20" xr:uid="{111B4475-977A-49B9-9657-CCB615DEF79F}"/>
+    <hyperlink ref="G49" r:id="rId21" xr:uid="{471A5D33-835A-414E-97B8-362512B11F19}"/>
+    <hyperlink ref="G50" r:id="rId22" xr:uid="{C7E5B850-A6A3-47EB-B6C2-A656ABE578C3}"/>
+    <hyperlink ref="H44" r:id="rId23" xr:uid="{57BA88B1-4374-4605-B1CF-000FB7A9AD17}"/>
+    <hyperlink ref="H45" r:id="rId24" xr:uid="{1020C407-DE4D-45CD-B802-7B6DA3235B83}"/>
+    <hyperlink ref="H46" r:id="rId25" xr:uid="{4A959DA8-94AE-478F-AA59-3FF5B726B06D}"/>
+    <hyperlink ref="H47" r:id="rId26" xr:uid="{A2EA3677-590B-439E-B26B-BBB5D057F411}"/>
+    <hyperlink ref="H48" r:id="rId27" xr:uid="{E55440CE-A9F7-403D-B428-B5518F503072}"/>
+    <hyperlink ref="H49" r:id="rId28" xr:uid="{A922F6B7-45E9-4EC5-85E8-E946899CA468}"/>
+    <hyperlink ref="H50" r:id="rId29" xr:uid="{0AF8DC04-D1CF-4807-A710-B373CBBE5749}"/>
+    <hyperlink ref="G51" r:id="rId30" xr:uid="{4930390E-877B-48E6-806D-25B7F1D8C5B8}"/>
+    <hyperlink ref="G52" r:id="rId31" xr:uid="{F7B5D713-A9B5-4133-BD07-98197D7E72D4}"/>
+    <hyperlink ref="G53" r:id="rId32" xr:uid="{E5AB4738-A96D-4977-A386-A581CA3C01E6}"/>
+    <hyperlink ref="G54" r:id="rId33" xr:uid="{DE1E9284-2F49-42F1-A7C3-B0CEC31B6EFD}"/>
+    <hyperlink ref="G55" r:id="rId34" xr:uid="{E2B9685A-2447-4FE1-AF1B-C87EA1440D7B}"/>
+    <hyperlink ref="H18:H42" r:id="rId35" display="Test@123" xr:uid="{428C5C26-7283-4267-926D-F8A15A909940}"/>
+    <hyperlink ref="H51:H55" r:id="rId36" display="Test@123" xr:uid="{1F19B917-4AC7-4318-9D2C-B3B3447CBA4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId50"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Structure search cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63F97D1-FDB9-421B-8F6E-53395FCB12D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2139C8D3-22E8-45D4-9E75-3412C2F9E3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="276">
   <si>
     <t>TSID</t>
   </si>
@@ -762,9 +762,6 @@
 Session ID: 53ad33f3cc438da53e2c48224f39c0fc</t>
   </si>
   <si>
-    <t>Rerun</t>
-  </si>
-  <si>
     <t>Fail:click on Button Tab Insights is not working for :: java.lang.NullPointerExceptionclick on Button Tab Insights is not working for :: java.lang.NullPointerException</t>
   </si>
   <si>
@@ -847,19 +844,6 @@
 *** Element info: {Using=xpath, value=//span[@class='mat-button-wrapper'][contains(.,'Clear all')]}</t>
   </si>
   <si>
-    <t xml:space="preserve">Fail:clickOnExpandDropdown is not working waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: (//section[@class='filter-details']//div[@class='mat-form-field-infix']//mat-icon)[1]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@cf08bec (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61364}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: a9c619a601bbd29729595f9063780838clickOnExpandDropdown is not working waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: (//section[@class='filter-details']//div[@class='mat-form-field-infix']//mat-icon)[1]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@cf08bec (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61364}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: a9c619a601bbd29729595f9063780838Results are not get refreshed </t>
-  </si>
-  <si>
     <t>Fail:PDF window opens has not opened</t>
   </si>
   <si>
@@ -976,6 +960,106 @@
   </si>
   <si>
     <t>Fail:setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' (tried for 50 second(s) with 500 milliseconds interval)setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' (tried for 50 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1291</t>
+  </si>
+  <si>
+    <t>validate Structure Search landing page and literature tab</t>
+  </si>
+  <si>
+    <t>validateStructureSearchAndLiteratureTab</t>
+  </si>
+  <si>
+    <t>ASPIRIN</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1292</t>
+  </si>
+  <si>
+    <t>validate phrase and keywords in restuls page for the structure search</t>
+  </si>
+  <si>
+    <t>validateStructureSearchKeywordsAndPhrase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antibacterial, polyethylene, resin </t>
+  </si>
+  <si>
+    <t>WATER</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1293</t>
+  </si>
+  <si>
+    <t>validate hit structure images and pagination</t>
+  </si>
+  <si>
+    <t>validateHitStructureImagesAndPagination</t>
+  </si>
+  <si>
+    <t>CN110343315A</t>
+  </si>
+  <si>
+    <t>Validate Chemical Structure filter Field</t>
+  </si>
+  <si>
+    <t>Validate ChemicalStructure Pagination And CheckboxSelection</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validate TextInputBox For Structure</t>
+  </si>
+  <si>
+    <t>CC(=O)OC1=CC=CC=C1C(=O)O</t>
+  </si>
+  <si>
+    <t>smiley</t>
+  </si>
+  <si>
+    <t>validateChemicalStructureFilterField</t>
+  </si>
+  <si>
+    <t>validateChemicalStructureFilterPaginationAndCheckboxSelection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> validateTextInputBoxForStructure</t>
+  </si>
+  <si>
+    <t>validateModifyChemicalStructureModal</t>
+  </si>
+  <si>
+    <t>Validate Modify Chemical StructureModal</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1346</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1347</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1348</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail:clickOnExpandDropdown is not working waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: (//section[@class='filter-details']//div[@class='mat-form-field-infix']//mat-icon)[1]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@ac9f52b (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.210', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61370}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: dde5f8da0abad15f5de451ac7fd9aaddclickOnExpandDropdown is not working waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: (//section[@class='filter-details']//div[@class='mat-form-field-infix']//mat-icon)[1]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@ac9f52b (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.210', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61370}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: dde5f8da0abad15f5de451ac7fd9aaddResults are not get refreshed </t>
+  </si>
+  <si>
+    <t>Rerun</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1126,6 +1210,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1136,7 +1231,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1187,6 +1282,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1574,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:XFD63"/>
+    <sheetView tabSelected="1" topLeftCell="G35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,10 +1690,13 @@
     <col min="10" max="10" width="40" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="14.7109375" style="4" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="8.85546875" style="4" collapsed="1"/>
+    <col min="13" max="13" width="8.85546875" style="4" collapsed="1"/>
+    <col min="14" max="14" width="28" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="27.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16384" width="8.85546875" style="4" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1640,8 +1739,11 @@
       <c r="N1" s="4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>82</v>
       </c>
@@ -1655,7 +1757,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F2" t="s">
         <v>221</v>
@@ -1670,7 +1772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>83</v>
       </c>
@@ -1684,10 +1786,10 @@
         <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>204</v>
@@ -1699,7 +1801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>84</v>
       </c>
@@ -1713,10 +1815,10 @@
         <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>204</v>
@@ -1728,7 +1830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>85</v>
       </c>
@@ -1742,10 +1844,10 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>204</v>
@@ -1757,7 +1859,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -1771,10 +1873,10 @@
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>204</v>
@@ -1786,7 +1888,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>87</v>
       </c>
@@ -1800,7 +1902,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F7" t="s">
         <v>176</v>
@@ -1818,7 +1920,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="255" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>88</v>
       </c>
@@ -1832,10 +1934,10 @@
         <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>204</v>
@@ -1850,7 +1952,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>89</v>
       </c>
@@ -1864,10 +1966,10 @@
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>204</v>
@@ -1882,7 +1984,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>90</v>
       </c>
@@ -1896,10 +1998,10 @@
         <v>40</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>204</v>
@@ -1911,7 +2013,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>91</v>
       </c>
@@ -1925,10 +2027,10 @@
         <v>43</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>204</v>
@@ -1943,7 +2045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>92</v>
       </c>
@@ -1957,7 +2059,7 @@
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F12" t="s">
         <v>176</v>
@@ -1975,7 +2077,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>94</v>
       </c>
@@ -1989,10 +2091,10 @@
         <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>204</v>
@@ -2007,7 +2109,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>95</v>
       </c>
@@ -2021,10 +2123,10 @@
         <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>204</v>
@@ -2039,7 +2141,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>96</v>
       </c>
@@ -2053,10 +2155,10 @@
         <v>52</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>204</v>
@@ -2071,7 +2173,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>97</v>
       </c>
@@ -2085,7 +2187,7 @@
         <v>61</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F16" t="s">
         <v>176</v>
@@ -2115,10 +2217,10 @@
         <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>199</v>
@@ -2146,7 +2248,7 @@
         <v>67</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>176</v>
@@ -2176,10 +2278,10 @@
         <v>64</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>222</v>
+        <v>275</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>233</v>
+        <v>274</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>199</v>
@@ -2207,7 +2309,7 @@
         <v>77</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>176</v>
@@ -2238,7 +2340,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>176</v>
@@ -2274,10 +2376,10 @@
         <v>75</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>199</v>
@@ -2305,10 +2407,10 @@
         <v>56</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>199</v>
@@ -2336,7 +2438,7 @@
         <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>176</v>
@@ -2364,7 +2466,7 @@
         <v>60</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>176</v>
@@ -2395,7 +2497,7 @@
         <v>79</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>176</v>
@@ -2426,7 +2528,7 @@
         <v>72</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>176</v>
@@ -2459,10 +2561,10 @@
         <v>112</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>199</v>
@@ -2488,7 +2590,7 @@
         <v>118</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>176</v>
@@ -2517,7 +2619,7 @@
         <v>121</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>176</v>
@@ -2546,10 +2648,10 @@
         <v>124</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>199</v>
@@ -2575,10 +2677,10 @@
         <v>126</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>199</v>
@@ -2604,7 +2706,7 @@
         <v>129</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>176</v>
@@ -2633,7 +2735,7 @@
         <v>132</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>176</v>
@@ -2662,7 +2764,7 @@
         <v>134</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>176</v>
@@ -2691,7 +2793,7 @@
         <v>136</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>176</v>
@@ -2721,7 +2823,7 @@
         <v>139</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F37" s="13" t="s">
         <v>176</v>
@@ -2751,7 +2853,7 @@
         <v>142</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F38" s="13" t="s">
         <v>176</v>
@@ -2781,7 +2883,7 @@
         <v>145</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F39" s="13" t="s">
         <v>176</v>
@@ -2811,7 +2913,7 @@
         <v>148</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>176</v>
@@ -2841,7 +2943,7 @@
         <v>151</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>176</v>
@@ -2870,7 +2972,7 @@
         <v>154</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>176</v>
@@ -2899,7 +3001,7 @@
         <v>156</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F43" t="s">
         <v>176</v>
@@ -2928,10 +3030,10 @@
         <v>159</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F44" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G44" s="18" t="s">
         <v>204</v>
@@ -2957,10 +3059,10 @@
         <v>161</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F45" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G45" s="18" t="s">
         <v>204</v>
@@ -2986,7 +3088,7 @@
         <v>162</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F46" t="s">
         <v>176</v>
@@ -3015,7 +3117,7 @@
         <v>164</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F47" t="s">
         <v>176</v>
@@ -3044,7 +3146,7 @@
         <v>166</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F48" t="s">
         <v>176</v>
@@ -3059,7 +3161,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>191</v>
       </c>
@@ -3073,10 +3175,10 @@
         <v>179</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F49" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G49" s="18" t="s">
         <v>204</v>
@@ -3088,7 +3190,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>192</v>
       </c>
@@ -3102,10 +3204,10 @@
         <v>182</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G50" s="24" t="s">
         <v>204</v>
@@ -3118,7 +3220,7 @@
       </c>
       <c r="J50" s="25"/>
     </row>
-    <row r="51" spans="1:13" s="12" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="12" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>193</v>
       </c>
@@ -3132,10 +3234,10 @@
         <v>184</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>199</v>
@@ -3151,7 +3253,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>194</v>
       </c>
@@ -3165,7 +3267,7 @@
         <v>187</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>176</v>
@@ -3180,7 +3282,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>195</v>
       </c>
@@ -3194,10 +3296,10 @@
         <v>189</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G53" s="18" t="s">
         <v>199</v>
@@ -3209,7 +3311,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>215</v>
       </c>
@@ -3223,10 +3325,10 @@
         <v>198</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G54" s="24" t="s">
         <v>199</v>
@@ -3239,7 +3341,7 @@
       </c>
       <c r="J54" s="25"/>
     </row>
-    <row r="55" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
         <v>216</v>
       </c>
@@ -3253,7 +3355,7 @@
         <v>201</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="F55" s="23" t="s">
         <v>176</v>
@@ -3269,7 +3371,7 @@
       </c>
       <c r="J55" s="25"/>
     </row>
-    <row r="56" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>210</v>
       </c>
@@ -3283,10 +3385,10 @@
         <v>203</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G56" s="22" t="s">
         <v>204</v>
@@ -3299,7 +3401,7 @@
       </c>
       <c r="J56" s="25"/>
     </row>
-    <row r="57" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>211</v>
       </c>
@@ -3313,10 +3415,10 @@
         <v>207</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F57" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G57" s="22" t="s">
         <v>204</v>
@@ -3329,7 +3431,7 @@
       </c>
       <c r="J57" s="25"/>
     </row>
-    <row r="58" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>212</v>
       </c>
@@ -3343,10 +3445,10 @@
         <v>209</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="F58" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G58" s="22" t="s">
         <v>204</v>
@@ -3358,6 +3460,236 @@
         <v>23</v>
       </c>
       <c r="J58" s="25"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H59" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="N59" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G60" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H60" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="N60" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G61" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H61" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="N62" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F63" t="s">
+        <v>176</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="N63" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F64" t="s">
+        <v>176</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N64" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G65" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="H65" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="N65" s="4" t="s">
+        <v>254</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M53" xr:uid="{EB08446A-0716-488E-B42E-00D2DA842126}"/>
@@ -3399,8 +3731,16 @@
     <hyperlink ref="G55" r:id="rId34" xr:uid="{E2B9685A-2447-4FE1-AF1B-C87EA1440D7B}"/>
     <hyperlink ref="H18:H42" r:id="rId35" display="Test@123" xr:uid="{428C5C26-7283-4267-926D-F8A15A909940}"/>
     <hyperlink ref="H51:H55" r:id="rId36" display="Test@123" xr:uid="{1F19B917-4AC7-4318-9D2C-B3B3447CBA4E}"/>
+    <hyperlink ref="G62" r:id="rId37" xr:uid="{C837631E-D83F-4CAB-B7EF-359AC0B72C2C}"/>
+    <hyperlink ref="G63" r:id="rId38" xr:uid="{B216E578-99F7-4539-95BC-CEAE985CF4A1}"/>
+    <hyperlink ref="G64" r:id="rId39" xr:uid="{1E1ADCC4-95BC-4AF8-9AB3-7EE388B85F1D}"/>
+    <hyperlink ref="G65" r:id="rId40" xr:uid="{C0E8DCD0-B5EB-40AA-B3E2-20F3244F6E65}"/>
+    <hyperlink ref="H62" r:id="rId41" xr:uid="{111BCB90-F2D5-450B-B749-7249F56DBF39}"/>
+    <hyperlink ref="H63" r:id="rId42" xr:uid="{29167A98-D6C2-4F18-BA83-7020E938AB86}"/>
+    <hyperlink ref="H64" r:id="rId43" xr:uid="{B0A91A7F-96A4-477C-9A31-4C51B69E3C70}"/>
+    <hyperlink ref="H65" r:id="rId44" xr:uid="{6DA28F36-CB17-4142-B2C8-A1F53BE08003}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId37"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ausust scope data updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7523612F-8F9D-494E-A778-187F42FF456B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E311762-5CD8-4583-9EB8-EBAAD6AD38FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="chemicalsearch" sheetId="80" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">chemicalsearch!$A$1:$M$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">chemicalsearch!$A$1:$M$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="292">
   <si>
     <t>TSID</t>
   </si>
@@ -774,19 +774,6 @@
     <t>Fail:nullnull</t>
   </si>
   <si>
-    <t>Fail:hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@37489e45 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60833}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 86aaf565f74f4903c6a42e2001cd98d1hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@37489e45 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60833}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 86aaf565f74f4903c6a42e2001cd98d1</t>
-  </si>
-  <si>
     <t>Fail:hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@206d7f15 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
@@ -1022,6 +1009,9 @@
     <t>validateChemicalStructureFilterField</t>
   </si>
   <si>
+    <t>validateChemicalStructureFilterPaginationAndCheckboxSelection</t>
+  </si>
+  <si>
     <t xml:space="preserve"> validateTextInputBoxForStructure</t>
   </si>
   <si>
@@ -1056,10 +1046,68 @@
 Session ID: dde5f8da0abad15f5de451ac7fd9aaddResults are not get refreshed </t>
   </si>
   <si>
-    <t>Rerun</t>
-  </si>
-  <si>
-    <t>validateChemicalStructureFilterPaginationAndCheckboxSelections</t>
+    <t>Validate - Resultset page - Company and Person search</t>
+  </si>
+  <si>
+    <t>one,two,three,four,five,six,seven,eight,nine,ten,one,two,three,four,five,six,seven,eight,nine,ten,one,two,three,four,five,six,seven,eight,nine,ten,one,two,three,four,five,six,seven,eight,nine,ten,one,two,three,four,five,six,seven,eight,nine</t>
+  </si>
+  <si>
+    <t>Fail:setKeyWords is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (4a6fdb9121a765c6b1efc64caccf97de)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@220e25fa (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.20.148', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 92.0.4515.107, chrome: {chromedriverVersion: 92.0.4515.107 (87a818b10553..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62818}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 4a6fdb9121a765c6b1efc64caccf97desetKeyWords is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (4a6fdb9121a765c6b1efc64caccf97de)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@220e25fa (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-84X6PV2', ip: '10.50.20.148', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 92.0.4515.107, chrome: {chromedriverVersion: 92.0.4515.107 (87a818b10553..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62818}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 4a6fdb9121a765c6b1efc64caccf97de</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vaildateCompanyPeopleSearchRSPage</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1590</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1569</t>
+  </si>
+  <si>
+    <t>Patent - validate customize cluster items</t>
+  </si>
+  <si>
+    <t>vaildatePatentClusterItems</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1570</t>
+  </si>
+  <si>
+    <t>Literature - validate customize cluster items</t>
+  </si>
+  <si>
+    <t>vaildateLiteratureClusterItems</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1567</t>
+  </si>
+  <si>
+    <t>Validate - Landing page - Company and Person search</t>
+  </si>
+  <si>
+    <t>vaildateCompanyPeopleSearch</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1568</t>
+  </si>
+  <si>
+    <t>Validate - Landing page - Company , Person search,Free text and Structure Search</t>
+  </si>
+  <si>
+    <t>vaildateCompanyPeoplePhraseStructureSearch</t>
+  </si>
+  <si>
+    <t>YN</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1279,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1283,6 +1331,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1670,10 +1721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1791,7 @@
         <v>220</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1757,7 +1808,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F2" t="s">
         <v>221</v>
@@ -1786,7 +1837,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>222</v>
@@ -1815,7 +1866,7 @@
         <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F4" t="s">
         <v>223</v>
@@ -1844,7 +1895,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F5" t="s">
         <v>224</v>
@@ -1873,7 +1924,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F6" t="s">
         <v>225</v>
@@ -1902,7 +1953,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F7" t="s">
         <v>176</v>
@@ -1934,10 +1985,10 @@
         <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>204</v>
@@ -1966,10 +2017,10 @@
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>204</v>
@@ -1998,10 +2049,10 @@
         <v>40</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>204</v>
@@ -2027,10 +2078,10 @@
         <v>43</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>204</v>
@@ -2059,7 +2110,7 @@
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F12" t="s">
         <v>176</v>
@@ -2091,10 +2142,10 @@
         <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>204</v>
@@ -2123,10 +2174,10 @@
         <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>204</v>
@@ -2155,7 +2206,7 @@
         <v>52</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F15" t="s">
         <v>225</v>
@@ -2187,7 +2238,7 @@
         <v>61</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F16" t="s">
         <v>176</v>
@@ -2217,10 +2268,10 @@
         <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>199</v>
@@ -2248,7 +2299,7 @@
         <v>67</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>176</v>
@@ -2278,7 +2329,7 @@
         <v>64</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>273</v>
@@ -2309,7 +2360,7 @@
         <v>77</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>176</v>
@@ -2340,7 +2391,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>176</v>
@@ -2376,10 +2427,10 @@
         <v>75</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>199</v>
@@ -2407,10 +2458,10 @@
         <v>56</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>199</v>
@@ -2438,7 +2489,7 @@
         <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>176</v>
@@ -2466,7 +2517,7 @@
         <v>60</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>176</v>
@@ -2497,7 +2548,7 @@
         <v>79</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>176</v>
@@ -2528,7 +2579,7 @@
         <v>72</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>176</v>
@@ -2561,10 +2612,10 @@
         <v>112</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>199</v>
@@ -2590,7 +2641,7 @@
         <v>118</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>176</v>
@@ -2619,7 +2670,7 @@
         <v>121</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>176</v>
@@ -2648,10 +2699,10 @@
         <v>124</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>199</v>
@@ -2677,10 +2728,10 @@
         <v>126</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>199</v>
@@ -2706,7 +2757,7 @@
         <v>129</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>176</v>
@@ -2735,7 +2786,7 @@
         <v>132</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>176</v>
@@ -2764,7 +2815,7 @@
         <v>134</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>176</v>
@@ -2793,7 +2844,7 @@
         <v>136</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>176</v>
@@ -2823,7 +2874,7 @@
         <v>139</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F37" s="13" t="s">
         <v>176</v>
@@ -2853,7 +2904,7 @@
         <v>142</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F38" s="13" t="s">
         <v>176</v>
@@ -2883,7 +2934,7 @@
         <v>145</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F39" s="13" t="s">
         <v>176</v>
@@ -2913,7 +2964,7 @@
         <v>148</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>176</v>
@@ -2943,7 +2994,7 @@
         <v>151</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>176</v>
@@ -2972,7 +3023,7 @@
         <v>154</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>176</v>
@@ -3001,7 +3052,7 @@
         <v>156</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F43" t="s">
         <v>176</v>
@@ -3030,10 +3081,10 @@
         <v>159</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F44" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G44" s="18" t="s">
         <v>204</v>
@@ -3059,10 +3110,10 @@
         <v>161</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G45" s="18" t="s">
         <v>204</v>
@@ -3088,7 +3139,7 @@
         <v>162</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>261</v>
+        <v>3</v>
       </c>
       <c r="F46" t="s">
         <v>176</v>
@@ -3117,7 +3168,7 @@
         <v>164</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F47" t="s">
         <v>176</v>
@@ -3146,7 +3197,7 @@
         <v>166</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F48" t="s">
         <v>176</v>
@@ -3175,10 +3226,10 @@
         <v>179</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F49" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G49" s="18" t="s">
         <v>204</v>
@@ -3204,10 +3255,10 @@
         <v>182</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G50" s="24" t="s">
         <v>204</v>
@@ -3234,10 +3285,10 @@
         <v>184</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>199</v>
@@ -3267,7 +3318,7 @@
         <v>187</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>176</v>
@@ -3296,10 +3347,10 @@
         <v>189</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G53" s="18" t="s">
         <v>199</v>
@@ -3325,10 +3376,10 @@
         <v>198</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G54" s="24" t="s">
         <v>199</v>
@@ -3355,7 +3406,7 @@
         <v>201</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F55" s="23" t="s">
         <v>176</v>
@@ -3385,10 +3436,10 @@
         <v>203</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G56" s="22" t="s">
         <v>204</v>
@@ -3415,10 +3466,10 @@
         <v>207</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F57" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G57" s="22" t="s">
         <v>204</v>
@@ -3445,10 +3496,10 @@
         <v>209</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F58" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G58" s="22" t="s">
         <v>204</v>
@@ -3463,19 +3514,19 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>248</v>
-      </c>
       <c r="E59" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>176</v>
@@ -3487,24 +3538,24 @@
         <v>205</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="C60" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>252</v>
-      </c>
       <c r="E60" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>176</v>
@@ -3519,27 +3570,27 @@
         <v>20</v>
       </c>
       <c r="J60" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N60" s="4" t="s">
         <v>253</v>
-      </c>
-      <c r="N60" s="4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="C61" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="22" t="s">
         <v>256</v>
       </c>
-      <c r="C61" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="22" t="s">
-        <v>257</v>
-      </c>
       <c r="E61" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>176</v>
@@ -3551,10 +3602,10 @@
         <v>205</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -3562,16 +3613,16 @@
         <v>269</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C62" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>176</v>
@@ -3586,10 +3637,10 @@
         <v>20</v>
       </c>
       <c r="J62" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N62" s="4" t="s">
         <v>253</v>
-      </c>
-      <c r="N62" s="4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -3597,7 +3648,7 @@
         <v>270</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C63" s="22" t="s">
         <v>14</v>
@@ -3606,7 +3657,7 @@
         <v>266</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F63" t="s">
         <v>176</v>
@@ -3618,10 +3669,10 @@
         <v>219</v>
       </c>
       <c r="N63" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -3638,7 +3689,7 @@
         <v>267</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F64" t="s">
         <v>176</v>
@@ -3653,7 +3704,7 @@
         <v>20</v>
       </c>
       <c r="N64" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -3661,16 +3712,16 @@
         <v>272</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C65" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>176</v>
@@ -3685,14 +3736,165 @@
         <v>20</v>
       </c>
       <c r="J65" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N65" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="N65" s="4" t="s">
-        <v>254</v>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H66" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="I66" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H67" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="I67" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G68" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H68" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="I68" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G69" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="I69" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="21" t="s">
+        <v>278</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="I70" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M53" xr:uid="{EB08446A-0716-488E-B42E-00D2DA842126}"/>
+  <autoFilter ref="A1:M70" xr:uid="{EB08446A-0716-488E-B42E-00D2DA842126}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G17" r:id="rId1" xr:uid="{723970F4-4603-469C-B45C-96036D0B804A}"/>
@@ -3739,8 +3941,10 @@
     <hyperlink ref="H63" r:id="rId42" xr:uid="{29167A98-D6C2-4F18-BA83-7020E938AB86}"/>
     <hyperlink ref="H64" r:id="rId43" xr:uid="{B0A91A7F-96A4-477C-9A31-4C51B69E3C70}"/>
     <hyperlink ref="H65" r:id="rId44" xr:uid="{6DA28F36-CB17-4142-B2C8-A1F53BE08003}"/>
+    <hyperlink ref="G70" r:id="rId45" xr:uid="{6303DB8D-1B7E-4608-812E-AB683479C51C}"/>
+    <hyperlink ref="H70" r:id="rId46" xr:uid="{3EC9ABF3-377B-46E8-8585-FD35C630B6C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId45"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UPdated the password for the user anand.perumallukamichetty@clarivate.com
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E311762-5CD8-4583-9EB8-EBAAD6AD38FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDD4775-2C07-48C3-B9F9-E117BE971738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Module" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="303">
   <si>
     <t>TSID</t>
   </si>
@@ -749,69 +749,6 @@
     <t>smiles</t>
   </si>
   <si>
-    <t>Fail:waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2e32a8c4 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61426}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 53ad33f3cc438da53e2c48224f39c0fcwaitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2e32a8c4 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61426}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 53ad33f3cc438da53e2c48224f39c0fc</t>
-  </si>
-  <si>
-    <t>Fail:click on Button Tab Insights is not working for :: java.lang.NullPointerExceptionclick on Button Tab Insights is not working for :: java.lang.NullPointerException</t>
-  </si>
-  <si>
-    <t>Fail:clickOnThumbsUpIcon is not workingjava.lang.NullPointerExceptionclickOnThumbsUpIcon is not workingjava.lang.NullPointerException</t>
-  </si>
-  <si>
-    <t>Fail:Title Field is not displayed for given row in Literature results page.Title is not displayed for given row in Patent results page.Patent tab is not displayed in results page.Literature tab is not displayed in results page.SearchBox is not displayed next to Liturature Tab.</t>
-  </si>
-  <si>
-    <t>Fail:nullnull</t>
-  </si>
-  <si>
-    <t>Fail:hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@206d7f15 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55555}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 8adf3a36bb0fca3958115472e66174e6hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@206d7f15 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55555}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 8adf3a36bb0fca3958115472e66174e6</t>
-  </si>
-  <si>
-    <t>Fail:Toast Message has not been displayed.Search box accepted morethan 2000 characters</t>
-  </si>
-  <si>
-    <t>Fail:getColorOfPillBox is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]"}
-  (Session info: chrome=91.0.4472.124)
-For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51235}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: d2275a66ca0ccabe24b119ce462f12d1
-*** Element info: {Using=xpath, value=(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]}getColorOfPillBox is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]"}
-  (Session info: chrome=91.0.4472.124)
-For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51235}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: d2275a66ca0ccabe24b119ce462f12d1
-*** Element info: {Using=xpath, value=(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]}</t>
-  </si>
-  <si>
-    <t>Fail:isDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerExceptionisDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerException</t>
-  </si>
-  <si>
     <t>Fail:ClearAll button is in disable modeclickOnbutton ClearAll Filters is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//span[@class='mat-button-wrapper'][contains(.,'Clear all')]"}
   (Session info: chrome=91.0.4472.124)
 For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
@@ -856,64 +793,6 @@
     <t>Fail:Inventor filter field  IS ENABLED</t>
   </si>
   <si>
-    <t>Fail:checkbox is not selectedjava.lang.Exception: jsClick is not  working on:: [[ChromeDriver: chrome on WINDOWS (9ef33598e97cc300166e18f03587e4d5)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on WINDOWS (9ef33598e97cc300166e18f03587e4d5)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57543}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 9ef33598e97cc300166e18f03587e4d5checkbox is not selectedjava.lang.Exception: jsClick is not  working on:: [[ChromeDriver: chrome on WINDOWS (9ef33598e97cc300166e18f03587e4d5)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on WINDOWS (9ef33598e97cc300166e18f03587e4d5)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57543}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 9ef33598e97cc300166e18f03587e4d5</t>
-  </si>
-  <si>
-    <t>Fail:checkbox is not selectedjava.lang.Exception: jsClick is not  working on:: [[ChromeDriver: chrome on WINDOWS (ac4881dbb7541956be0c94efa15cb71a)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on WINDOWS (ac4881dbb7541956be0c94efa15cb71a)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55134}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: ac4881dbb7541956be0c94efa15cb71acheckbox is not selectedjava.lang.Exception: jsClick is not  working on:: [[ChromeDriver: chrome on WINDOWS (ac4881dbb7541956be0c94efa15cb71a)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on WINDOWS (ac4881dbb7541956be0c94efa15cb71a)] -&gt; xpath: //div[contains(text(),'Publication year')]/ancestor::mat-expansion-panel-header/following-sibling::div//mat-selection-list[@role='list']/mat-list-item[@role='listitem'][19]] (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55134}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: ac4881dbb7541956be0c94efa15cb71a</t>
-  </si>
-  <si>
-    <t>Fail:RESULT SETS ARE NOT REFRESHED  : 	28551		 AFTER FILTER :	154waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; aside &gt; div:nth-child(1) &gt; span.pn' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@27de4165 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63655}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: b7c44885cd7be62fb773220e779c505bwaitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; aside &gt; div:nth-child(1) &gt; span.pn' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@27de4165 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63655}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: b7c44885cd7be62fb773220e779c505b</t>
-  </si>
-  <si>
-    <t>Fail:getTextLiteratureTitle is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"css selector","selector":"app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-header &gt; div &gt; mat-card-subtitle"}
-  (Session info: chrome=91.0.4472.124)
-For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56914}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: c9f312d12df25e39d309a236c704c38d
-*** Element info: {Using=css selector, value=app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-header &gt; div &gt; mat-card-subtitle}getTextLiteratureTitle is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"css selector","selector":"app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-header &gt; div &gt; mat-card-subtitle"}
-  (Session info: chrome=91.0.4472.124)
-For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56914}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: c9f312d12df25e39d309a236c704c38d
-*** Element info: {Using=css selector, value=app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-header &gt; div &gt; mat-card-subtitle}</t>
-  </si>
-  <si>
     <t>Fail:clickOnMoreFiltersDropdown is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@class='mat-select-arrow']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@40a1ff79 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
@@ -933,22 +812,6 @@
     <t>Fail:setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-placeholder='Type folder name']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-placeholder='Type folder name']' (tried for 50 second(s) with 500 milliseconds interval)setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-placeholder='Type folder name']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-placeholder='Type folder name']' (tried for 50 second(s) with 500 milliseconds interval)</t>
   </si>
   <si>
-    <t>Fail:clickOnCitingPatentViewASResultSet is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (26a2606bc0f59e6c132214108e51d4a9)] -&gt; xpath: (//span[contains(.,'View as result set')])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@34fa4ff7 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50777}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 26a2606bc0f59e6c132214108e51d4a9clickOnCitingPatentViewASResultSet is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (26a2606bc0f59e6c132214108e51d4a9)] -&gt; xpath: (//span[contains(.,'View as result set')])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@34fa4ff7 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.80.222', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 91.0.4472.124, chrome: {chromedriverVersion: 91.0.4472.101 (af52a90bf870..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50777}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 26a2606bc0f59e6c132214108e51d4a9</t>
-  </si>
-  <si>
-    <t>Fail:setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' (tried for 50 second(s) with 500 milliseconds interval)setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //input[@ng-reflect-maxlength='150']' (tried for 50 second(s) with 500 milliseconds interval)</t>
-  </si>
-  <si>
     <t>CHEMEXP-1291</t>
   </si>
   <si>
@@ -992,9 +855,6 @@
   </si>
   <si>
     <t>Validate ChemicalStructure Pagination And CheckboxSelection</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t xml:space="preserve"> Validate TextInputBox For Structure</t>
@@ -1052,19 +912,6 @@
     <t>one,two,three,four,five,six,seven,eight,nine,ten,one,two,three,four,five,six,seven,eight,nine,ten,one,two,three,four,five,six,seven,eight,nine,ten,one,two,three,four,five,six,seven,eight,nine,ten,one,two,three,four,five,six,seven,eight,nine</t>
   </si>
   <si>
-    <t>Fail:setKeyWords is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (4a6fdb9121a765c6b1efc64caccf97de)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@220e25fa (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.20.148', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 92.0.4515.107, chrome: {chromedriverVersion: 92.0.4515.107 (87a818b10553..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62818}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 4a6fdb9121a765c6b1efc64caccf97desetKeyWords is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (4a6fdb9121a765c6b1efc64caccf97de)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@220e25fa (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-84X6PV2', ip: '10.50.20.148', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_91'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 92.0.4515.107, chrome: {chromedriverVersion: 92.0.4515.107 (87a818b10553..., userDataDir: C:\Users\U6049848\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62818}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 4a6fdb9121a765c6b1efc64caccf97de</t>
-  </si>
-  <si>
     <t xml:space="preserve"> vaildateCompanyPeopleSearchRSPage</t>
   </si>
   <si>
@@ -1107,7 +954,303 @@
     <t>vaildateCompanyPeoplePhraseStructureSearch</t>
   </si>
   <si>
-    <t>YN</t>
+    <t>Derwent@12345</t>
+  </si>
+  <si>
+    <t>Fail:isDisabledSearchIcon is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[1]/div[3]/button[2]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@109ab414 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57008}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: fdbe747cfb6309788ca62290cbddcddcisDisabledSearchIcon is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[1]/div[3]/button[2]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@109ab414 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57008}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: fdbe747cfb6309788ca62290cbddcddc</t>
+  </si>
+  <si>
+    <t>Fail:click on Button Tab Insights is not working for :: java.lang.NullPointerExceptionclick on Button Tab Insights is not working for :: java.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>Fail:clickOnThumbsUpIcon is not workingjava.lang.NullPointerExceptionclickOnThumbsUpIcon is not workingjava.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>Fail:Title Field is not displayed for given row in Literature results page.Title is not displayed for given row in Patent results page.Patent tab is not displayed in results page.Literature tab is not displayed in results page.SearchBox is not displayed next to Liturature Tab.</t>
+  </si>
+  <si>
+    <t>Fail:nullnull</t>
+  </si>
+  <si>
+    <t>Fail:newly entered keyword :acidic should not converted into a pill</t>
+  </si>
+  <si>
+    <t>Fail:New keywords are not entered.hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@127446dc (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57548}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: b465634bca51c9a60e1bd03f368697c5hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@127446dc (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57548}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: b465634bca51c9a60e1bd03f368697c5</t>
+  </si>
+  <si>
+    <t>Fail:hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3a69593c (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:54006}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 889586bf755fddc5f2b8d9c8b9c54464hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3a69593c (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:54006}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 889586bf755fddc5f2b8d9c8b9c54464</t>
+  </si>
+  <si>
+    <t>Fail:Search box accepted morethan 2000 characters</t>
+  </si>
+  <si>
+    <t>Fail:Looking Pillbox doesnot exist in result setgetColorOfPillBox is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]"}
+  (Session info: headless chrome=93.0.4577.63)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53816}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 5be4a5f6f592b7c8d7d2b3b926035af2
+*** Element info: {Using=xpath, value=(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]}getColorOfPillBox is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]"}
+  (Session info: headless chrome=93.0.4577.63)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53816}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 5be4a5f6f592b7c8d7d2b3b926035af2
+*** Element info: {Using=xpath, value=(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]}</t>
+  </si>
+  <si>
+    <t>Fail:waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (fa18703d5f0e3dd6f46aa28866ab55de)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@362d1ce7 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57821}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: fa18703d5f0e3dd6f46aa28866ab55dewaitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (fa18703d5f0e3dd6f46aa28866ab55de)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@362d1ce7 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57821}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: fa18703d5f0e3dd6f46aa28866ab55de</t>
+  </si>
+  <si>
+    <t>Fail:isDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerExceptionisDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>Fail:waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (e25f55cd55729c81585d60fff1251498)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@488017a4 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:49676}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: e25f55cd55729c81585d60fff1251498waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (e25f55cd55729c81585d60fff1251498)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@488017a4 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:49676}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: e25f55cd55729c81585d60fff1251498</t>
+  </si>
+  <si>
+    <t>Fail:clickOnPillBox is not working..org.openqa.selenium.ElementNotInteractableException: element not interactable
+  (Session info: headless chrome=93.0.4577.63)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62596}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 5c84c7f72128f173ffad7d47d4c57a3aclickOnPillBox is not working..org.openqa.selenium.ElementNotInteractableException: element not interactable
+  (Session info: headless chrome=93.0.4577.63)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62596}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 5c84c7f72128f173ffad7d47d4c57a3a</t>
+  </si>
+  <si>
+    <t>Fail: java.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //body[contains(text(),'PDF is not available')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@47845f69 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53676}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 77b9426541fe4ad3bc7257c974b986a1 java.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //body[contains(text(),'PDF is not available')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@47845f69 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53676}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 77b9426541fe4ad3bc7257c974b986a1</t>
+  </si>
+  <si>
+    <t>Fail:clickOnSupportLink is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: div.links &gt; button:nth-child(5) &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1e16ab3e (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58173}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 7756071bbfc460fae11187f5a2a0dbdfclickOnSupportLink is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: div.links &gt; button:nth-child(5) &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1e16ab3e (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58173}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 7756071bbfc460fae11187f5a2a0dbdf</t>
+  </si>
+  <si>
+    <t>Fail:deSelectMultiplePublicationChartFilters is not working..org.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;rect width="12.138728323699421" height="50.98926187481861" x="126.58959537572255" y="69.01073812518139" id="publ_year_rect_2007" class="rect-selected" style="fill: rgb(0, 60, 143);"&gt;&lt;/rect&gt; is not clickable at point (1695, 413). Other element would receive the click: &lt;line stroke="currentColor" x2="-300"&gt;&lt;/line&gt;
+  (Session info: headless chrome=93.0.4577.63)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50291}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: cbf7c180b471c0c2015182f9db78a162deSelectMultiplePublicationChartFilters is not working..org.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;rect width="12.138728323699421" height="50.98926187481861" x="126.58959537572255" y="69.01073812518139" id="publ_year_rect_2007" class="rect-selected" style="fill: rgb(0, 60, 143);"&gt;&lt;/rect&gt; is not clickable at point (1695, 413). Other element would receive the click: &lt;line stroke="currentColor" x2="-300"&gt;&lt;/line&gt;
+  (Session info: headless chrome=93.0.4577.63)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50291}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: cbf7c180b471c0c2015182f9db78a162</t>
+  </si>
+  <si>
+    <t>Fail:checkbox is not selectedjava.lang.Exception: clickOn filter is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//span[@class='mat-content']//div[contains(text(),'Publication year')]"}
+  (Session info: headless chrome=93.0.4577.63)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56223}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a1455fa65d2a79024db57f2b5da88e64
+*** Element info: {Using=xpath, value=//span[@class='mat-content']//div[contains(text(),'Publication year')]}checkbox is not selectedjava.lang.Exception: clickOn filter is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//span[@class='mat-content']//div[contains(text(),'Publication year')]"}
+  (Session info: headless chrome=93.0.4577.63)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56223}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a1455fa65d2a79024db57f2b5da88e64
+*** Element info: {Using=xpath, value=//span[@class='mat-content']//div[contains(text(),'Publication year')]}</t>
+  </si>
+  <si>
+    <t>Fail:setTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath:  //textarea[@placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@27f3afde (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61822}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: c2b4e9ded61cc45ceab44206710237cdsetTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath:  //textarea[@placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@27f3afde (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61822}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: c2b4e9ded61cc45ceab44206710237cd</t>
+  </si>
+  <si>
+    <t>Fail:SMALL SIZE IMAGE IS NOT DISPLAYED IN RSMEDIUM SIZE IMAGE IS NOT DISPLAYED IN RSLARGE SIZE IMAGE IS NOT DISPLAYED IN RS</t>
+  </si>
+  <si>
+    <t>Fail:clickOnLinkAssignee is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section &gt; app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; div:nth-child(1) &gt; section.assignee.ng-star-inserted &gt; p &gt; span &gt; span &gt; a' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@61ea3f67 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58596}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 74e21b0aba45c5587fec2b6eca0e9773clickOnLinkAssignee is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section &gt; app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; div:nth-child(1) &gt; section.assignee.ng-star-inserted &gt; p &gt; span &gt; span &gt; a' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@61ea3f67 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58596}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 74e21b0aba45c5587fec2b6eca0e9773</t>
+  </si>
+  <si>
+    <t>Fail:clickOnLinkMoreLikeThis is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; section:nth-child(3) &gt; div &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@346509dd (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63599}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 65a75ed2c022287d76bb5dcd9a59f9f3clickOnLinkMoreLikeThis is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; section:nth-child(3) &gt; div &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@346509dd (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63599}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 65a75ed2c022287d76bb5dcd9a59f9f3</t>
+  </si>
+  <si>
+    <t>Fail:clickOnLinkCreateNewFolder is not workingorg.openqa.selenium.json.JsonException: java.lang.reflect.InvocationTargetException
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: driver.version: RemoteWebDriverclickOnLinkCreateNewFolder is not workingorg.openqa.selenium.json.JsonException: java.lang.reflect.InvocationTargetException
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: driver.version: RemoteWebDriver</t>
+  </si>
+  <si>
+    <t>Fail:clickOnRSFooterGlobalCheckBox is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //app-result-paginator-bar/section[1]/span[1]/mat-checkbox/label/div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@72b7c29f (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63523}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 19573ec23fd3afee5cfff66d2cdba866clickOnRSFooterGlobalCheckBox is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //app-result-paginator-bar/section[1]/span[1]/mat-checkbox/label/div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@72b7c29f (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63523}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 19573ec23fd3afee5cfff66d2cdba866</t>
+  </si>
+  <si>
+    <t>Fail:waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@41cb9225 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52962}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 4ada26358cc134f14f3a82b8ffbf2949waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@41cb9225 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52962}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 4ada26358cc134f14f3a82b8ffbf2949</t>
+  </si>
+  <si>
+    <t>Fail:getTextImageViewerPaginatorRange is not workingjava.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div/mat-dialog-content/section/div[2]/div[2]/mat-paginator/div/div/div/div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3bdebf49 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60079}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 7f16670eec8d4f5ee2cf798745980c35getTextImageViewerPaginatorRange is not workingjava.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div/mat-dialog-content/section/div[2]/div[2]/mat-paginator/div/div/div/div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3bdebf49 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60079}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 7f16670eec8d4f5ee2cf798745980c35</t>
+  </si>
+  <si>
+    <t>Fail:setTextPersonOrOrganization is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //input[contains(@placeholder,'Enter name')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@717e34b5 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55239}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: fae33f2de9f91536050b414cb9d5df58setTextPersonOrOrganization is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //input[contains(@placeholder,'Enter name')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@717e34b5 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55239}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: fae33f2de9f91536050b414cb9d5df58</t>
+  </si>
+  <si>
+    <t>Fail:setTextPersonOrOrganization is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //input[contains(@placeholder,'Enter name')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@7ba2a1cd (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58068}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 58cb19a0b87afdb4b326c088dd9b29b8setTextPersonOrOrganization is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //input[contains(@placeholder,'Enter name')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@7ba2a1cd (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58068}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 58cb19a0b87afdb4b326c088dd9b29b8</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1258,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1272,14 +1415,14 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1334,6 +1477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1685,14 +1829,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" width="25.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1703,7 +1847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1723,31 +1867,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="65.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.6640625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65.88671875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.6640625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="59" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.77734375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="255" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="70.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.33203125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="70.44140625" style="4" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="40" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.85546875" style="4" collapsed="1"/>
+    <col min="11" max="11" width="14.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8.88671875" style="4" collapsed="1"/>
     <col min="14" max="14" width="28" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="27.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16384" width="8.85546875" style="4" collapsed="1"/>
+    <col min="15" max="15" width="27.44140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16384" width="8.88671875" style="4" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1791,10 +1935,10 @@
         <v>220</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>82</v>
       </c>
@@ -1808,22 +1952,22 @@
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>221</v>
+        <v>275</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>205</v>
+      <c r="H2" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>83</v>
       </c>
@@ -1837,22 +1981,22 @@
         <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>222</v>
+        <v>276</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>205</v>
+      <c r="H3" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>84</v>
       </c>
@@ -1866,22 +2010,22 @@
         <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>223</v>
+        <v>277</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>205</v>
+      <c r="H4" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>85</v>
       </c>
@@ -1895,22 +2039,22 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>224</v>
+        <v>278</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>205</v>
+      <c r="H5" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -1924,22 +2068,22 @@
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>225</v>
+        <v>279</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>205</v>
+      <c r="H6" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>87</v>
       </c>
@@ -1953,16 +2097,16 @@
         <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>176</v>
+        <v>280</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>205</v>
+      <c r="H7" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>31</v>
@@ -1971,7 +2115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="255" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>88</v>
       </c>
@@ -1985,16 +2129,16 @@
         <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>205</v>
+      <c r="H8" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>35</v>
@@ -2003,7 +2147,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>89</v>
       </c>
@@ -2017,16 +2161,16 @@
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>226</v>
+        <v>282</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>205</v>
+      <c r="H9" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>35</v>
@@ -2035,7 +2179,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>90</v>
       </c>
@@ -2049,22 +2193,22 @@
         <v>40</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>227</v>
+        <v>283</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>205</v>
+      <c r="H10" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>91</v>
       </c>
@@ -2078,16 +2222,16 @@
         <v>43</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>228</v>
+        <v>284</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>205</v>
+      <c r="H11" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>20</v>
@@ -2096,7 +2240,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>92</v>
       </c>
@@ -2110,16 +2254,16 @@
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>176</v>
+        <v>285</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>205</v>
+      <c r="H12" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>20</v>
@@ -2128,7 +2272,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>94</v>
       </c>
@@ -2142,16 +2286,16 @@
         <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>229</v>
+        <v>286</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>205</v>
+      <c r="H13" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>20</v>
@@ -2160,7 +2304,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>95</v>
       </c>
@@ -2174,16 +2318,16 @@
         <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>229</v>
+        <v>287</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>205</v>
+      <c r="H14" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>20</v>
@@ -2192,7 +2336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>96</v>
       </c>
@@ -2206,16 +2350,16 @@
         <v>52</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>225</v>
+        <v>288</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>205</v>
+      <c r="H15" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>35</v>
@@ -2224,7 +2368,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>97</v>
       </c>
@@ -2238,23 +2382,23 @@
         <v>61</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>176</v>
+        <v>289</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>205</v>
+      <c r="H16" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I16" s="27" t="s">
         <v>218</v>
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:12" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>98</v>
       </c>
@@ -2268,10 +2412,10 @@
         <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>199</v>
@@ -2285,7 +2429,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>99</v>
       </c>
@@ -2299,7 +2443,7 @@
         <v>67</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>176</v>
@@ -2315,7 +2459,7 @@
       </c>
       <c r="J18" s="11"/>
     </row>
-    <row r="19" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>100</v>
       </c>
@@ -2329,10 +2473,10 @@
         <v>64</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>199</v>
@@ -2346,7 +2490,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
     </row>
-    <row r="20" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>101</v>
       </c>
@@ -2360,7 +2504,7 @@
         <v>77</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>176</v>
@@ -2377,7 +2521,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
     </row>
-    <row r="21" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>102</v>
       </c>
@@ -2391,7 +2535,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>176</v>
@@ -2413,7 +2557,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>105</v>
       </c>
@@ -2427,10 +2571,10 @@
         <v>75</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>199</v>
@@ -2444,7 +2588,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="1:12" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>107</v>
       </c>
@@ -2458,10 +2602,10 @@
         <v>56</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>199</v>
@@ -2475,7 +2619,7 @@
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
     </row>
-    <row r="24" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>108</v>
       </c>
@@ -2489,7 +2633,7 @@
         <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>176</v>
@@ -2503,7 +2647,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
     </row>
-    <row r="25" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>109</v>
       </c>
@@ -2517,7 +2661,7 @@
         <v>60</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>176</v>
@@ -2534,7 +2678,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:12" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>110</v>
       </c>
@@ -2548,7 +2692,7 @@
         <v>79</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>176</v>
@@ -2565,7 +2709,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
     </row>
-    <row r="27" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>111</v>
       </c>
@@ -2579,7 +2723,7 @@
         <v>72</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>176</v>
@@ -2598,7 +2742,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>113</v>
       </c>
@@ -2612,10 +2756,10 @@
         <v>112</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>199</v>
@@ -2627,7 +2771,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>116</v>
       </c>
@@ -2641,7 +2785,7 @@
         <v>118</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>176</v>
@@ -2656,7 +2800,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>119</v>
       </c>
@@ -2670,7 +2814,7 @@
         <v>121</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>176</v>
@@ -2685,7 +2829,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>122</v>
       </c>
@@ -2699,10 +2843,10 @@
         <v>124</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>199</v>
@@ -2714,7 +2858,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>125</v>
       </c>
@@ -2728,10 +2872,10 @@
         <v>126</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>199</v>
@@ -2743,7 +2887,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>127</v>
       </c>
@@ -2757,7 +2901,7 @@
         <v>129</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>176</v>
@@ -2772,7 +2916,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="99.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>130</v>
       </c>
@@ -2786,7 +2930,7 @@
         <v>132</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>176</v>
@@ -2801,7 +2945,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>133</v>
       </c>
@@ -2815,7 +2959,7 @@
         <v>134</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>176</v>
@@ -2830,7 +2974,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>135</v>
       </c>
@@ -2844,7 +2988,7 @@
         <v>136</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>176</v>
@@ -2860,7 +3004,7 @@
       </c>
       <c r="J36" s="13"/>
     </row>
-    <row r="37" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>137</v>
       </c>
@@ -2874,7 +3018,7 @@
         <v>139</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F37" s="13" t="s">
         <v>176</v>
@@ -2890,7 +3034,7 @@
       </c>
       <c r="J37" s="13"/>
     </row>
-    <row r="38" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>140</v>
       </c>
@@ -2904,7 +3048,7 @@
         <v>142</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F38" s="13" t="s">
         <v>176</v>
@@ -2920,7 +3064,7 @@
       </c>
       <c r="J38" s="13"/>
     </row>
-    <row r="39" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>143</v>
       </c>
@@ -2934,7 +3078,7 @@
         <v>145</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F39" s="13" t="s">
         <v>176</v>
@@ -2950,7 +3094,7 @@
       </c>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>146</v>
       </c>
@@ -2964,7 +3108,7 @@
         <v>148</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>176</v>
@@ -2980,7 +3124,7 @@
       </c>
       <c r="J40" s="13"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>149</v>
       </c>
@@ -2994,7 +3138,7 @@
         <v>151</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>176</v>
@@ -3009,7 +3153,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>152</v>
       </c>
@@ -3023,7 +3167,7 @@
         <v>154</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>176</v>
@@ -3038,7 +3182,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>167</v>
       </c>
@@ -3052,22 +3196,22 @@
         <v>156</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F43" t="s">
-        <v>176</v>
+        <v>290</v>
       </c>
       <c r="G43" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H43" s="18" t="s">
-        <v>205</v>
+      <c r="H43" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>168</v>
       </c>
@@ -3081,22 +3225,22 @@
         <v>159</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F44" t="s">
-        <v>236</v>
+        <v>291</v>
       </c>
       <c r="G44" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H44" s="18" t="s">
-        <v>205</v>
+      <c r="H44" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>169</v>
       </c>
@@ -3110,22 +3254,22 @@
         <v>161</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F45" t="s">
-        <v>237</v>
+        <v>292</v>
       </c>
       <c r="G45" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H45" s="18" t="s">
-        <v>205</v>
+      <c r="H45" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>170</v>
       </c>
@@ -3142,7 +3286,7 @@
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>176</v>
+        <v>293</v>
       </c>
       <c r="G46" s="18" t="s">
         <v>204</v>
@@ -3154,7 +3298,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>171</v>
       </c>
@@ -3168,7 +3312,7 @@
         <v>164</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F47" t="s">
         <v>176</v>
@@ -3176,14 +3320,14 @@
       <c r="G47" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H47" s="18" t="s">
-        <v>205</v>
+      <c r="H47" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>172</v>
       </c>
@@ -3197,22 +3341,22 @@
         <v>166</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F48" t="s">
-        <v>176</v>
+        <v>294</v>
       </c>
       <c r="G48" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H48" s="18" t="s">
-        <v>205</v>
+      <c r="H48" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>191</v>
       </c>
@@ -3226,22 +3370,22 @@
         <v>179</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>238</v>
+        <v>295</v>
       </c>
       <c r="G49" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H49" s="18" t="s">
-        <v>205</v>
+      <c r="H49" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
         <v>192</v>
       </c>
@@ -3255,23 +3399,23 @@
         <v>182</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>239</v>
+        <v>296</v>
       </c>
       <c r="G50" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="H50" s="24" t="s">
-        <v>205</v>
+      <c r="H50" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I50" s="22" t="s">
         <v>20</v>
       </c>
       <c r="J50" s="25"/>
     </row>
-    <row r="51" spans="1:15" s="12" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="12" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>193</v>
       </c>
@@ -3285,10 +3429,10 @@
         <v>184</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>199</v>
@@ -3304,7 +3448,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>194</v>
       </c>
@@ -3318,7 +3462,7 @@
         <v>187</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>176</v>
@@ -3333,7 +3477,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>195</v>
       </c>
@@ -3347,10 +3491,10 @@
         <v>189</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="G53" s="18" t="s">
         <v>199</v>
@@ -3362,7 +3506,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="21" t="s">
         <v>215</v>
       </c>
@@ -3376,10 +3520,10 @@
         <v>198</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="G54" s="24" t="s">
         <v>199</v>
@@ -3392,7 +3536,7 @@
       </c>
       <c r="J54" s="25"/>
     </row>
-    <row r="55" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="21" t="s">
         <v>216</v>
       </c>
@@ -3406,7 +3550,7 @@
         <v>201</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F55" s="23" t="s">
         <v>176</v>
@@ -3422,7 +3566,7 @@
       </c>
       <c r="J55" s="25"/>
     </row>
-    <row r="56" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="21" t="s">
         <v>210</v>
       </c>
@@ -3436,23 +3580,23 @@
         <v>203</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="F56" s="22" t="s">
-        <v>243</v>
+        <v>3</v>
+      </c>
+      <c r="F56" t="s">
+        <v>228</v>
       </c>
       <c r="G56" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H56" s="22" t="s">
-        <v>205</v>
+      <c r="H56" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I56" s="26" t="s">
         <v>214</v>
       </c>
       <c r="J56" s="25"/>
     </row>
-    <row r="57" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="21" t="s">
         <v>211</v>
       </c>
@@ -3466,23 +3610,23 @@
         <v>207</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="F57" s="22" t="s">
-        <v>244</v>
+        <v>3</v>
+      </c>
+      <c r="F57" t="s">
+        <v>297</v>
       </c>
       <c r="G57" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H57" s="22" t="s">
-        <v>205</v>
+      <c r="H57" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I57" s="22" t="s">
         <v>20</v>
       </c>
       <c r="J57" s="25"/>
     </row>
-    <row r="58" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="21" t="s">
         <v>212</v>
       </c>
@@ -3496,37 +3640,37 @@
         <v>209</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="F58" s="22" t="s">
-        <v>244</v>
+        <v>3</v>
+      </c>
+      <c r="F58" t="s">
+        <v>298</v>
       </c>
       <c r="G58" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H58" s="22" t="s">
-        <v>205</v>
+      <c r="H58" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I58" s="22" t="s">
         <v>23</v>
       </c>
       <c r="J58" s="25"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="21" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="C59" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>176</v>
@@ -3534,95 +3678,95 @@
       <c r="G59" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H59" s="22" t="s">
-        <v>205</v>
+      <c r="H59" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="21" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="C60" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>176</v>
+        <v>299</v>
       </c>
       <c r="G60" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H60" s="22" t="s">
-        <v>205</v>
+      <c r="H60" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>20</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="21" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C61" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>176</v>
+        <v>300</v>
       </c>
       <c r="G61" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H61" s="22" t="s">
-        <v>205</v>
+      <c r="H61" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="N61" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62" s="21" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="21" t="s">
-        <v>269</v>
-      </c>
       <c r="B62" s="4" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="C62" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>176</v>
@@ -3637,27 +3781,27 @@
         <v>20</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="21" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="C63" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F63" t="s">
         <v>176</v>
@@ -3669,27 +3813,27 @@
         <v>219</v>
       </c>
       <c r="N63" s="28" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="21" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F64" t="s">
         <v>176</v>
@@ -3704,24 +3848,24 @@
         <v>20</v>
       </c>
       <c r="N64" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="21" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C65" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>176</v>
@@ -3736,27 +3880,27 @@
         <v>20</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="21" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="C66" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>291</v>
+        <v>3</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>176</v>
@@ -3764,28 +3908,28 @@
       <c r="G66" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H66" s="22" t="s">
-        <v>205</v>
+      <c r="H66" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I66" s="22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="C67" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>291</v>
+        <v>3</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>176</v>
@@ -3793,86 +3937,86 @@
       <c r="G67" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H67" s="22" t="s">
-        <v>205</v>
+      <c r="H67" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I67" s="22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="21" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="C68" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>291</v>
+        <v>3</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>176</v>
+        <v>301</v>
       </c>
       <c r="G68" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H68" s="22" t="s">
-        <v>205</v>
+      <c r="H68" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I68" s="22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="21" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="C69" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>291</v>
+        <v>3</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>176</v>
+        <v>302</v>
       </c>
       <c r="G69" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="H69" s="22" t="s">
-        <v>205</v>
+      <c r="H69" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="I69" s="22" t="s">
         <v>23</v>
       </c>
       <c r="N69" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A70" s="21" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C70" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>3</v>
@@ -3890,7 +4034,7 @@
         <v>115</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3911,40 +4055,33 @@
     <hyperlink ref="G41" r:id="rId12" xr:uid="{F030BE8B-BC36-49E1-8D71-1478C5C4BCDF}"/>
     <hyperlink ref="G42" r:id="rId13" xr:uid="{23135E44-8E96-4D83-A082-A7511C1C0771}"/>
     <hyperlink ref="G43" r:id="rId14" xr:uid="{0CCCEC04-DDD0-4D0F-8D23-C47F6F6CEC53}"/>
-    <hyperlink ref="H43" r:id="rId15" xr:uid="{D41C1E47-89D1-498E-802F-F4AA544A235B}"/>
-    <hyperlink ref="G44" r:id="rId16" xr:uid="{D466216C-1EF1-4553-A660-7BF606C27DB9}"/>
-    <hyperlink ref="G45" r:id="rId17" xr:uid="{F86289C3-3FA2-4BA4-AEDD-552CD06D34E6}"/>
-    <hyperlink ref="G46" r:id="rId18" xr:uid="{0DE6A34B-2C8E-4613-99BD-7169693A3191}"/>
-    <hyperlink ref="G47" r:id="rId19" xr:uid="{0E6F7DF1-DD17-41D2-B68A-807CE6F4A387}"/>
-    <hyperlink ref="G48" r:id="rId20" xr:uid="{111B4475-977A-49B9-9657-CCB615DEF79F}"/>
-    <hyperlink ref="G49" r:id="rId21" xr:uid="{471A5D33-835A-414E-97B8-362512B11F19}"/>
-    <hyperlink ref="G50" r:id="rId22" xr:uid="{C7E5B850-A6A3-47EB-B6C2-A656ABE578C3}"/>
-    <hyperlink ref="H44" r:id="rId23" xr:uid="{57BA88B1-4374-4605-B1CF-000FB7A9AD17}"/>
-    <hyperlink ref="H45" r:id="rId24" xr:uid="{1020C407-DE4D-45CD-B802-7B6DA3235B83}"/>
-    <hyperlink ref="H46" r:id="rId25" xr:uid="{4A959DA8-94AE-478F-AA59-3FF5B726B06D}"/>
-    <hyperlink ref="H47" r:id="rId26" xr:uid="{A2EA3677-590B-439E-B26B-BBB5D057F411}"/>
-    <hyperlink ref="H48" r:id="rId27" xr:uid="{E55440CE-A9F7-403D-B428-B5518F503072}"/>
-    <hyperlink ref="H49" r:id="rId28" xr:uid="{A922F6B7-45E9-4EC5-85E8-E946899CA468}"/>
-    <hyperlink ref="H50" r:id="rId29" xr:uid="{0AF8DC04-D1CF-4807-A710-B373CBBE5749}"/>
-    <hyperlink ref="G51" r:id="rId30" xr:uid="{4930390E-877B-48E6-806D-25B7F1D8C5B8}"/>
-    <hyperlink ref="G52" r:id="rId31" xr:uid="{F7B5D713-A9B5-4133-BD07-98197D7E72D4}"/>
-    <hyperlink ref="G53" r:id="rId32" xr:uid="{E5AB4738-A96D-4977-A386-A581CA3C01E6}"/>
-    <hyperlink ref="G54" r:id="rId33" xr:uid="{DE1E9284-2F49-42F1-A7C3-B0CEC31B6EFD}"/>
-    <hyperlink ref="G55" r:id="rId34" xr:uid="{E2B9685A-2447-4FE1-AF1B-C87EA1440D7B}"/>
-    <hyperlink ref="H18:H42" r:id="rId35" display="Test@123" xr:uid="{428C5C26-7283-4267-926D-F8A15A909940}"/>
-    <hyperlink ref="H51:H55" r:id="rId36" display="Test@123" xr:uid="{1F19B917-4AC7-4318-9D2C-B3B3447CBA4E}"/>
-    <hyperlink ref="G62" r:id="rId37" xr:uid="{C837631E-D83F-4CAB-B7EF-359AC0B72C2C}"/>
-    <hyperlink ref="G63" r:id="rId38" xr:uid="{B216E578-99F7-4539-95BC-CEAE985CF4A1}"/>
-    <hyperlink ref="G64" r:id="rId39" xr:uid="{1E1ADCC4-95BC-4AF8-9AB3-7EE388B85F1D}"/>
-    <hyperlink ref="G65" r:id="rId40" xr:uid="{C0E8DCD0-B5EB-40AA-B3E2-20F3244F6E65}"/>
-    <hyperlink ref="H62" r:id="rId41" xr:uid="{111BCB90-F2D5-450B-B749-7249F56DBF39}"/>
-    <hyperlink ref="H63" r:id="rId42" xr:uid="{29167A98-D6C2-4F18-BA83-7020E938AB86}"/>
-    <hyperlink ref="H64" r:id="rId43" xr:uid="{B0A91A7F-96A4-477C-9A31-4C51B69E3C70}"/>
-    <hyperlink ref="H65" r:id="rId44" xr:uid="{6DA28F36-CB17-4142-B2C8-A1F53BE08003}"/>
-    <hyperlink ref="G70" r:id="rId45" xr:uid="{6303DB8D-1B7E-4608-812E-AB683479C51C}"/>
-    <hyperlink ref="H70" r:id="rId46" xr:uid="{3EC9ABF3-377B-46E8-8585-FD35C630B6C3}"/>
+    <hyperlink ref="G44" r:id="rId15" xr:uid="{D466216C-1EF1-4553-A660-7BF606C27DB9}"/>
+    <hyperlink ref="G45" r:id="rId16" xr:uid="{F86289C3-3FA2-4BA4-AEDD-552CD06D34E6}"/>
+    <hyperlink ref="G46" r:id="rId17" xr:uid="{0DE6A34B-2C8E-4613-99BD-7169693A3191}"/>
+    <hyperlink ref="G47" r:id="rId18" xr:uid="{0E6F7DF1-DD17-41D2-B68A-807CE6F4A387}"/>
+    <hyperlink ref="G48" r:id="rId19" xr:uid="{111B4475-977A-49B9-9657-CCB615DEF79F}"/>
+    <hyperlink ref="G49" r:id="rId20" xr:uid="{471A5D33-835A-414E-97B8-362512B11F19}"/>
+    <hyperlink ref="G50" r:id="rId21" xr:uid="{C7E5B850-A6A3-47EB-B6C2-A656ABE578C3}"/>
+    <hyperlink ref="H46" r:id="rId22" xr:uid="{4A959DA8-94AE-478F-AA59-3FF5B726B06D}"/>
+    <hyperlink ref="G51" r:id="rId23" xr:uid="{4930390E-877B-48E6-806D-25B7F1D8C5B8}"/>
+    <hyperlink ref="G52" r:id="rId24" xr:uid="{F7B5D713-A9B5-4133-BD07-98197D7E72D4}"/>
+    <hyperlink ref="G53" r:id="rId25" xr:uid="{E5AB4738-A96D-4977-A386-A581CA3C01E6}"/>
+    <hyperlink ref="G54" r:id="rId26" xr:uid="{DE1E9284-2F49-42F1-A7C3-B0CEC31B6EFD}"/>
+    <hyperlink ref="G55" r:id="rId27" xr:uid="{E2B9685A-2447-4FE1-AF1B-C87EA1440D7B}"/>
+    <hyperlink ref="H18:H42" r:id="rId28" display="Test@123" xr:uid="{428C5C26-7283-4267-926D-F8A15A909940}"/>
+    <hyperlink ref="H51:H55" r:id="rId29" display="Test@123" xr:uid="{1F19B917-4AC7-4318-9D2C-B3B3447CBA4E}"/>
+    <hyperlink ref="G62" r:id="rId30" xr:uid="{C837631E-D83F-4CAB-B7EF-359AC0B72C2C}"/>
+    <hyperlink ref="G63" r:id="rId31" xr:uid="{B216E578-99F7-4539-95BC-CEAE985CF4A1}"/>
+    <hyperlink ref="G64" r:id="rId32" xr:uid="{1E1ADCC4-95BC-4AF8-9AB3-7EE388B85F1D}"/>
+    <hyperlink ref="G65" r:id="rId33" xr:uid="{C0E8DCD0-B5EB-40AA-B3E2-20F3244F6E65}"/>
+    <hyperlink ref="H62" r:id="rId34" xr:uid="{111BCB90-F2D5-450B-B749-7249F56DBF39}"/>
+    <hyperlink ref="H63" r:id="rId35" xr:uid="{29167A98-D6C2-4F18-BA83-7020E938AB86}"/>
+    <hyperlink ref="H64" r:id="rId36" xr:uid="{B0A91A7F-96A4-477C-9A31-4C51B69E3C70}"/>
+    <hyperlink ref="H65" r:id="rId37" xr:uid="{6DA28F36-CB17-4142-B2C8-A1F53BE08003}"/>
+    <hyperlink ref="G70" r:id="rId38" xr:uid="{6303DB8D-1B7E-4608-812E-AB683479C51C}"/>
+    <hyperlink ref="H70" r:id="rId39" xr:uid="{3EC9ABF3-377B-46E8-8585-FD35C630B6C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId47"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pushed code for CHEMEXP-1664 and CHEMEXP-1665
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDD4775-2C07-48C3-B9F9-E117BE971738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45CCCA9-1B19-4DB0-881B-A46315491FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="chemicalsearch" sheetId="80" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">chemicalsearch!$A$1:$M$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">chemicalsearch!$A$1:$M$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="307">
   <si>
     <t>TSID</t>
   </si>
@@ -957,61 +957,51 @@
     <t>Derwent@12345</t>
   </si>
   <si>
-    <t>Fail:isDisabledSearchIcon is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[1]/div[3]/button[2]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@109ab414 (tried for 50 second(s) with 500 milliseconds interval)
+    <t>Fail:clickOnThumbsUpIcon is not workingjava.lang.NullPointerExceptionclickOnThumbsUpIcon is not workingjava.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>Fail:Title Field is not displayed for given row in Literature results page.Title is not displayed for given row in Patent results page.Patent tab is not displayed in results page.Literature tab is not displayed in results page.SearchBox is not displayed next to Liturature Tab.</t>
+  </si>
+  <si>
+    <t>Fail:nullnull</t>
+  </si>
+  <si>
+    <t>Fail:Search box accepted morethan 2000 characters</t>
+  </si>
+  <si>
+    <t>Fail:SMALL SIZE IMAGE IS NOT DISPLAYED IN RSMEDIUM SIZE IMAGE IS NOT DISPLAYED IN RSLARGE SIZE IMAGE IS NOT DISPLAYED IN RS</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Fail:newly entered keyword :acidic should not converted into a pillResult set isnot get refreshed with new keyword</t>
+  </si>
+  <si>
+    <t>Fail:New keywords are not entered.hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@184be21a (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57008}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: fdbe747cfb6309788ca62290cbddcddcisDisabledSearchIcon is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[1]/div[3]/button[2]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@109ab414 (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:65424}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 3c49f8594f985885d0bd9eafd548348fhoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@184be21a (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57008}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: fdbe747cfb6309788ca62290cbddcddc</t>
-  </si>
-  <si>
-    <t>Fail:click on Button Tab Insights is not working for :: java.lang.NullPointerExceptionclick on Button Tab Insights is not working for :: java.lang.NullPointerException</t>
-  </si>
-  <si>
-    <t>Fail:clickOnThumbsUpIcon is not workingjava.lang.NullPointerExceptionclickOnThumbsUpIcon is not workingjava.lang.NullPointerException</t>
-  </si>
-  <si>
-    <t>Fail:Title Field is not displayed for given row in Literature results page.Title is not displayed for given row in Patent results page.Patent tab is not displayed in results page.Literature tab is not displayed in results page.SearchBox is not displayed next to Liturature Tab.</t>
-  </si>
-  <si>
-    <t>Fail:nullnull</t>
-  </si>
-  <si>
-    <t>Fail:newly entered keyword :acidic should not converted into a pill</t>
-  </si>
-  <si>
-    <t>Fail:New keywords are not entered.hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@127446dc (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:65424}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 3c49f8594f985885d0bd9eafd548348f</t>
+  </si>
+  <si>
+    <t>Fail:hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@7e56c5c (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57548}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: b465634bca51c9a60e1bd03f368697c5hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@127446dc (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53089}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 23c9e315f614ff5c0f5c5359756da5f1hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@7e56c5c (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57548}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: b465634bca51c9a60e1bd03f368697c5</t>
-  </si>
-  <si>
-    <t>Fail:hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3a69593c (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:54006}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 889586bf755fddc5f2b8d9c8b9c54464hoverOnPhraseSection is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3a69593c (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:54006}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 889586bf755fddc5f2b8d9c8b9c54464</t>
-  </si>
-  <si>
-    <t>Fail:Search box accepted morethan 2000 characters</t>
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53089}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 23c9e315f614ff5c0f5c5359756da5f1</t>
   </si>
   <si>
     <t>Fail:Looking Pillbox doesnot exist in result setgetColorOfPillBox is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]"}
@@ -1020,46 +1010,46 @@
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53816}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 5be4a5f6f592b7c8d7d2b3b926035af2
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:49694}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a9308dd5ffe76514a8dba49f9aa53ab7
 *** Element info: {Using=xpath, value=(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]}getColorOfPillBox is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]"}
   (Session info: headless chrome=93.0.4577.63)
 For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53816}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 5be4a5f6f592b7c8d7d2b3b926035af2
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:49694}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a9308dd5ffe76514a8dba49f9aa53ab7
 *** Element info: {Using=xpath, value=(//mat-chip[contains(@class,'mat-chip mat-primary mat-standard-chip')])[1]}</t>
   </si>
   <si>
-    <t>Fail:waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (fa18703d5f0e3dd6f46aa28866ab55de)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@362d1ce7 (tried for 50 second(s) with 500 milliseconds interval)
+    <t>Fail:waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (ce92e637393d96104a9241a4c32bb011)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2d7e304a (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57821}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: fa18703d5f0e3dd6f46aa28866ab55dewaitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (fa18703d5f0e3dd6f46aa28866ab55de)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@362d1ce7 (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62965}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: ce92e637393d96104a9241a4c32bb011waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (ce92e637393d96104a9241a4c32bb011)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2d7e304a (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57821}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: fa18703d5f0e3dd6f46aa28866ab55de</t>
-  </si>
-  <si>
-    <t>Fail:isDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerExceptionisDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerException</t>
-  </si>
-  <si>
-    <t>Fail:waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (e25f55cd55729c81585d60fff1251498)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@488017a4 (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62965}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: ce92e637393d96104a9241a4c32bb011</t>
+  </si>
+  <si>
+    <t>Fail:Result set is not get refreshed with new searchisDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerExceptionisDisplayedButtonThumsDownWithFillColor is not working..java.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>Fail:waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (762d5b41b465111960aab0415b97e673)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@616aa883 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:49676}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: e25f55cd55729c81585d60fff1251498waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (e25f55cd55729c81585d60fff1251498)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@488017a4 (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55595}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 762d5b41b465111960aab0415b97e673waitUntilElementIsDisplayed is not working.. :: [[ChromeDriver: chrome on WINDOWS (762d5b41b465111960aab0415b97e673)] -&gt; xpath: (//span[@class='cdx-chip-name'])[1]] org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@616aa883 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:49676}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: e25f55cd55729c81585d60fff1251498</t>
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55595}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 762d5b41b465111960aab0415b97e673</t>
   </si>
   <si>
     <t>Fail:clickOnPillBox is not working..org.openqa.selenium.ElementNotInteractableException: element not interactable
@@ -1067,40 +1057,40 @@
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62596}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 5c84c7f72128f173ffad7d47d4c57a3aclickOnPillBox is not working..org.openqa.selenium.ElementNotInteractableException: element not interactable
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50492}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 219d13d7ce975b7bc2044fa4329895ccclickOnPillBox is not working..org.openqa.selenium.ElementNotInteractableException: element not interactable
   (Session info: headless chrome=93.0.4577.63)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62596}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 5c84c7f72128f173ffad7d47d4c57a3a</t>
-  </si>
-  <si>
-    <t>Fail: java.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //body[contains(text(),'PDF is not available')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@47845f69 (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50492}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 219d13d7ce975b7bc2044fa4329895cc</t>
+  </si>
+  <si>
+    <t>Fail: java.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //body[contains(text(),'PDF is not available')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@104b49e0 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53676}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 77b9426541fe4ad3bc7257c974b986a1 java.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //body[contains(text(),'PDF is not available')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@47845f69 (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53236}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 491cd7d607374905ad4b467b5144cd35 java.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //body[contains(text(),'PDF is not available')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@104b49e0 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53676}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 77b9426541fe4ad3bc7257c974b986a1</t>
-  </si>
-  <si>
-    <t>Fail:clickOnSupportLink is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: div.links &gt; button:nth-child(5) &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1e16ab3e (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53236}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 491cd7d607374905ad4b467b5144cd35</t>
+  </si>
+  <si>
+    <t>Fail:clickOnSupportLink is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: div.links &gt; button:nth-child(5) &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2f667c7b (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58173}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 7756071bbfc460fae11187f5a2a0dbdfclickOnSupportLink is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: div.links &gt; button:nth-child(5) &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1e16ab3e (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56804}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 87703db48a3eaf37357a20f4eb385dabclickOnSupportLink is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: div.links &gt; button:nth-child(5) &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2f667c7b (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58173}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 7756071bbfc460fae11187f5a2a0dbdf</t>
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56804}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 87703db48a3eaf37357a20f4eb385dab</t>
   </si>
   <si>
     <t>Fail:deSelectMultiplePublicationChartFilters is not working..org.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;rect width="12.138728323699421" height="50.98926187481861" x="126.58959537572255" y="69.01073812518139" id="publ_year_rect_2007" class="rect-selected" style="fill: rgb(0, 60, 143);"&gt;&lt;/rect&gt; is not clickable at point (1695, 413). Other element would receive the click: &lt;line stroke="currentColor" x2="-300"&gt;&lt;/line&gt;
@@ -1108,14 +1098,14 @@
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50291}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: cbf7c180b471c0c2015182f9db78a162deSelectMultiplePublicationChartFilters is not working..org.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;rect width="12.138728323699421" height="50.98926187481861" x="126.58959537572255" y="69.01073812518139" id="publ_year_rect_2007" class="rect-selected" style="fill: rgb(0, 60, 143);"&gt;&lt;/rect&gt; is not clickable at point (1695, 413). Other element would receive the click: &lt;line stroke="currentColor" x2="-300"&gt;&lt;/line&gt;
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63395}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 3bbca2dfb9bd114db6beebad99cc384adeSelectMultiplePublicationChartFilters is not working..org.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;rect width="12.138728323699421" height="50.98926187481861" x="126.58959537572255" y="69.01073812518139" id="publ_year_rect_2007" class="rect-selected" style="fill: rgb(0, 60, 143);"&gt;&lt;/rect&gt; is not clickable at point (1695, 413). Other element would receive the click: &lt;line stroke="currentColor" x2="-300"&gt;&lt;/line&gt;
   (Session info: headless chrome=93.0.4577.63)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50291}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: cbf7c180b471c0c2015182f9db78a162</t>
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63395}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 3bbca2dfb9bd114db6beebad99cc384a</t>
   </si>
   <si>
     <t>Fail:checkbox is not selectedjava.lang.Exception: clickOn filter is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//span[@class='mat-content']//div[contains(text(),'Publication year')]"}
@@ -1124,133 +1114,99 @@
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56223}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: a1455fa65d2a79024db57f2b5da88e64
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56746}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 99ea0994bd2094813fd0191d790af2a5
 *** Element info: {Using=xpath, value=//span[@class='mat-content']//div[contains(text(),'Publication year')]}checkbox is not selectedjava.lang.Exception: clickOn filter is not workingorg.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//span[@class='mat-content']//div[contains(text(),'Publication year')]"}
   (Session info: headless chrome=93.0.4577.63)
 For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56223}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: a1455fa65d2a79024db57f2b5da88e64
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56746}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 99ea0994bd2094813fd0191d790af2a5
 *** Element info: {Using=xpath, value=//span[@class='mat-content']//div[contains(text(),'Publication year')]}</t>
   </si>
   <si>
-    <t>Fail:setTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath:  //textarea[@placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@27f3afde (tried for 50 second(s) with 500 milliseconds interval)
+    <t>Fail:setTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath:  //textarea[@placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@a8be31e (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61822}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: c2b4e9ded61cc45ceab44206710237cdsetTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath:  //textarea[@placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@27f3afde (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52093}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 25191c37b3b4da6f60ea6c0a74dc6ac7setTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath:  //textarea[@placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@a8be31e (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:61822}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: c2b4e9ded61cc45ceab44206710237cd</t>
-  </si>
-  <si>
-    <t>Fail:SMALL SIZE IMAGE IS NOT DISPLAYED IN RSMEDIUM SIZE IMAGE IS NOT DISPLAYED IN RSLARGE SIZE IMAGE IS NOT DISPLAYED IN RS</t>
-  </si>
-  <si>
-    <t>Fail:clickOnLinkAssignee is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section &gt; app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; div:nth-child(1) &gt; section.assignee.ng-star-inserted &gt; p &gt; span &gt; span &gt; a' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@61ea3f67 (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52093}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 25191c37b3b4da6f60ea6c0a74dc6ac7</t>
+  </si>
+  <si>
+    <t>Fail:clickOnLinkAssignee is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section &gt; app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; div:nth-child(1) &gt; section.assignee.ng-star-inserted &gt; p &gt; span &gt; span &gt; a' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1db2e6ec (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58596}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 74e21b0aba45c5587fec2b6eca0e9773clickOnLinkAssignee is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section &gt; app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; div:nth-child(1) &gt; section.assignee.ng-star-inserted &gt; p &gt; span &gt; span &gt; a' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@61ea3f67 (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62494}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a99599a7c83212a1f30010d71cbb314fclickOnLinkAssignee is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section &gt; app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; div:nth-child(1) &gt; section.assignee.ng-star-inserted &gt; p &gt; span &gt; span &gt; a' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1db2e6ec (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58596}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 74e21b0aba45c5587fec2b6eca0e9773</t>
-  </si>
-  <si>
-    <t>Fail:clickOnLinkMoreLikeThis is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; section:nth-child(3) &gt; div &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@346509dd (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:62494}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a99599a7c83212a1f30010d71cbb314f</t>
+  </si>
+  <si>
+    <t>Fail:clickOnLinkMoreLikeThis is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; section:nth-child(3) &gt; div &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3ab000a9 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63599}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 65a75ed2c022287d76bb5dcd9a59f9f3clickOnLinkMoreLikeThis is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; section:nth-child(3) &gt; div &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@346509dd (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56523}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: c53e1c2b25197039ff6375c6af5aa8d8clickOnLinkMoreLikeThis is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: app-result-set:nth-child(1) &gt; section &gt; mat-card &gt; mat-card-content &gt; section:nth-child(3) &gt; div &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3ab000a9 (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63599}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 65a75ed2c022287d76bb5dcd9a59f9f3</t>
-  </si>
-  <si>
-    <t>Fail:clickOnLinkCreateNewFolder is not workingorg.openqa.selenium.json.JsonException: java.lang.reflect.InvocationTargetException
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: driver.version: RemoteWebDriverclickOnLinkCreateNewFolder is not workingorg.openqa.selenium.json.JsonException: java.lang.reflect.InvocationTargetException
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: driver.version: RemoteWebDriver</t>
-  </si>
-  <si>
-    <t>Fail:clickOnRSFooterGlobalCheckBox is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //app-result-paginator-bar/section[1]/span[1]/mat-checkbox/label/div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@72b7c29f (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56523}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: c53e1c2b25197039ff6375c6af5aa8d8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail:CLEAR ALL ICON (X)IS DISPLAYED </t>
+  </si>
+  <si>
+    <t>Fail:isDisabledImageViewerNextPageArrow is not workingjava.lang.NullPointerExceptionisDisabledImageViewerNextPageArrow is not workingjava.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>Fail:setTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath:  //textarea[@placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2f78fd0e (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63523}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 19573ec23fd3afee5cfff66d2cdba866clickOnRSFooterGlobalCheckBox is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //app-result-paginator-bar/section[1]/span[1]/mat-checkbox/label/div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@72b7c29f (tried for 50 second(s) with 500 milliseconds interval)
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:54283}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 01a1cc1c4d5c18f8bdd21c519f5a0218setTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath:  //textarea[@placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@2f78fd0e (tried for 50 second(s) with 500 milliseconds interval)
 Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
 System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
 Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63523}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 19573ec23fd3afee5cfff66d2cdba866</t>
-  </si>
-  <si>
-    <t>Fail:waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@41cb9225 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52962}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 4ada26358cc134f14f3a82b8ffbf2949waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@ng-reflect-maxlength='2000']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@41cb9225 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52962}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 4ada26358cc134f14f3a82b8ffbf2949</t>
-  </si>
-  <si>
-    <t>Fail:getTextImageViewerPaginatorRange is not workingjava.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div/mat-dialog-content/section/div[2]/div[2]/mat-paginator/div/div/div/div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3bdebf49 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60079}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 7f16670eec8d4f5ee2cf798745980c35getTextImageViewerPaginatorRange is not workingjava.lang.Exception: getText is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div/mat-dialog-content/section/div[2]/div[2]/mat-paginator/div/div/div/div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@3bdebf49 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60079}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 7f16670eec8d4f5ee2cf798745980c35</t>
-  </si>
-  <si>
-    <t>Fail:setTextPersonOrOrganization is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //input[contains(@placeholder,'Enter name')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@717e34b5 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55239}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: fae33f2de9f91536050b414cb9d5df58setTextPersonOrOrganization is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //input[contains(@placeholder,'Enter name')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@717e34b5 (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:55239}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: fae33f2de9f91536050b414cb9d5df58</t>
-  </si>
-  <si>
-    <t>Fail:setTextPersonOrOrganization is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //input[contains(@placeholder,'Enter name')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@7ba2a1cd (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58068}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 58cb19a0b87afdb4b326c088dd9b29b8setTextPersonOrOrganization is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //input[contains(@placeholder,'Enter name')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@7ba2a1cd (tried for 50 second(s) with 500 milliseconds interval)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.15 (660fc11082ba5..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:58068}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 58cb19a0b87afdb4b326c088dd9b29b8</t>
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 93.0.4577.63, chrome: {chromedriverVersion: 93.0.4577.63 (ff5c0da2ec0ad..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:54283}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 01a1cc1c4d5c18f8bdd21c519f5a0218</t>
+  </si>
+  <si>
+    <t>Fail:setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //section[3]/form/section[1]/mat-form-field/div/div[1]/div[3]/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //section[3]/form/section[1]/mat-form-field/div/div[1]/div[3]/input' (tried for 50 second(s) with 500 milliseconds interval)setTextFolderName is not working..java.lang.Exception: selenium click is not  working on:: Proxy element for: DefaultElementLocator 'By.xpath: //section[3]/form/section[1]/mat-form-field/div/div[1]/div[3]/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLocator 'By.xpath: //section[3]/form/section[1]/mat-form-field/div/div[1]/div[3]/input' (tried for 50 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>Fail:User can not see 10 records per pageUser can not see 20 records per pageUser can not see 100 records per page</t>
+  </si>
+  <si>
+    <t>Validate annotation in RS and Saved Records Page</t>
+  </si>
+  <si>
+    <t>vaildateAnnotationResultSetAndSavedRecord</t>
+  </si>
+  <si>
+    <t>Validate annotation in Saved Folder and Saved Records Page</t>
+  </si>
+  <si>
+    <t>vaildateAnnotationSavedFolderAndSavedRecord</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1665</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1664</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1216,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1331,14 +1287,6 @@
       <family val="3"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
@@ -1378,7 +1326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1401,28 +1349,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1451,40 +1387,31 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="6" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="6" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma 2 2" xfId="3" xr:uid="{AA68FCC1-0F32-4B18-9A9A-444BEC9A472A}"/>
     <cellStyle name="Comma 2 2 2" xfId="5" xr:uid="{1A7BAE10-D655-46A3-884E-7A3BE33A8E6A}"/>
     <cellStyle name="Comma 2 3" xfId="4" xr:uid="{02E4C50F-082B-4B45-BB33-E0B251D59FE1}"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
@@ -1865,10 +1792,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="G67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1928,13 +1855,13 @@
       <c r="L1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="15" t="s">
         <v>247</v>
       </c>
     </row>
@@ -1952,15 +1879,15 @@
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>275</v>
+        <v>280</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I2" s="4" t="s">
@@ -1981,15 +1908,15 @@
         <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>276</v>
+        <v>176</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -2010,15 +1937,15 @@
         <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>277</v>
+        <v>280</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>275</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -2039,18 +1966,18 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>278</v>
+        <v>280</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>276</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="21" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2068,15 +1995,15 @@
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>279</v>
+        <v>280</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>277</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -2097,15 +2024,15 @@
         <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>280</v>
+        <v>280</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>281</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -2129,15 +2056,15 @@
         <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -2161,15 +2088,15 @@
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>282</v>
+        <v>280</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I9" s="5" t="s">
@@ -2193,15 +2120,15 @@
         <v>40</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>283</v>
+        <v>280</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>278</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -2222,15 +2149,15 @@
         <v>43</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" t="s">
+        <v>280</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>284</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I11" s="4" t="s">
@@ -2254,15 +2181,15 @@
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" t="s">
+        <v>280</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>285</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I12" s="4" t="s">
@@ -2286,15 +2213,15 @@
         <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" t="s">
+        <v>280</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>286</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I13" s="5" t="s">
@@ -2318,15 +2245,15 @@
         <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>287</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I14" s="5" t="s">
@@ -2350,15 +2277,15 @@
         <v>52</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" t="s">
+        <v>280</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>288</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -2382,18 +2309,18 @@
         <v>61</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" t="s">
+        <v>280</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>289</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="22" t="s">
         <v>218</v>
       </c>
       <c r="K16" s="2"/>
@@ -2412,15 +2339,15 @@
         <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I17" s="10" t="s">
@@ -2443,15 +2370,15 @@
         <v>67</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I18" s="11" t="s">
@@ -2473,15 +2400,15 @@
         <v>64</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I19" s="10" t="s">
@@ -2504,15 +2431,15 @@
         <v>77</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I20" s="10" t="s">
@@ -2535,15 +2462,15 @@
         <v>69</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I21" s="10" t="s">
@@ -2571,15 +2498,15 @@
         <v>75</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I22" s="10" t="s">
@@ -2602,22 +2529,22 @@
         <v>56</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
     </row>
     <row r="24" spans="1:12" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
@@ -2633,15 +2560,15 @@
         <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="20" t="s">
         <v>219</v>
       </c>
       <c r="J24" s="11"/>
@@ -2661,15 +2588,15 @@
         <v>60</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I25" s="10" t="s">
@@ -2692,15 +2619,15 @@
         <v>79</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G26" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I26" s="10" t="s">
@@ -2723,15 +2650,15 @@
         <v>72</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I27" s="10" t="s">
@@ -2756,15 +2683,15 @@
         <v>112</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="G28" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I28" s="4" t="s">
@@ -2785,15 +2712,15 @@
         <v>118</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="G29" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H29" s="18" t="s">
+      <c r="H29" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I29" s="4" t="s">
@@ -2814,15 +2741,15 @@
         <v>121</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G30" s="18" t="s">
+      <c r="G30" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H30" s="18" t="s">
+      <c r="H30" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I30" s="4" t="s">
@@ -2843,15 +2770,15 @@
         <v>124</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H31" s="18" t="s">
+      <c r="H31" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I31" s="4" t="s">
@@ -2872,15 +2799,15 @@
         <v>126</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I32" s="4" t="s">
@@ -2901,15 +2828,15 @@
         <v>129</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G33" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I33" s="4" t="s">
@@ -2930,15 +2857,15 @@
         <v>132</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G34" s="18" t="s">
+      <c r="G34" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H34" s="18" t="s">
+      <c r="H34" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I34" s="4" t="s">
@@ -2959,15 +2886,15 @@
         <v>134</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G35" s="18" t="s">
+      <c r="G35" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H35" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I35" s="4" t="s">
@@ -2988,15 +2915,15 @@
         <v>136</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G36" s="18" t="s">
+      <c r="G36" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I36" s="12" t="s">
@@ -3018,15 +2945,15 @@
         <v>139</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F37" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G37" s="18" t="s">
+      <c r="G37" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H37" s="18" t="s">
+      <c r="H37" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I37" s="12" t="s">
@@ -3048,15 +2975,15 @@
         <v>142</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F38" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G38" s="18" t="s">
+      <c r="G38" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I38" s="12" t="s">
@@ -3078,15 +3005,15 @@
         <v>145</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F39" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G39" s="18" t="s">
+      <c r="G39" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="H39" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I39" s="12" t="s">
@@ -3108,15 +3035,15 @@
         <v>148</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G40" s="18" t="s">
+      <c r="G40" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I40" s="12" t="s">
@@ -3138,15 +3065,15 @@
         <v>151</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G41" s="18" t="s">
+      <c r="G41" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H41" s="18" t="s">
+      <c r="H41" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I41" s="12" t="s">
@@ -3167,15 +3094,15 @@
         <v>154</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G42" s="18" t="s">
+      <c r="G42" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H42" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I42" s="12" t="s">
@@ -3196,15 +3123,15 @@
         <v>156</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
+        <v>280</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="G43" s="18" t="s">
+      <c r="G43" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I43" s="4" t="s">
@@ -3225,15 +3152,15 @@
         <v>159</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44" t="s">
+        <v>280</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="G44" s="18" t="s">
+      <c r="G44" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="H44" s="30" t="s">
+      <c r="H44" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I44" s="4" t="s">
@@ -3254,15 +3181,15 @@
         <v>161</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F45" t="s">
+        <v>280</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="G45" s="18" t="s">
+      <c r="G45" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="H45" s="30" t="s">
+      <c r="H45" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I45" s="4" t="s">
@@ -3283,15 +3210,15 @@
         <v>162</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F46" t="s">
+        <v>280</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="G46" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H46" s="20" t="s">
         <v>205</v>
       </c>
       <c r="I46" s="4" t="s">
@@ -3312,15 +3239,15 @@
         <v>164</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F47" t="s">
+        <v>280</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G47" s="18" t="s">
+      <c r="G47" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="H47" s="30" t="s">
+      <c r="H47" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I47" s="4" t="s">
@@ -3341,15 +3268,15 @@
         <v>166</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F48" t="s">
-        <v>294</v>
-      </c>
-      <c r="G48" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="G48" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="H48" s="30" t="s">
+      <c r="H48" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I48" s="4" t="s">
@@ -3370,50 +3297,50 @@
         <v>179</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F49" t="s">
-        <v>295</v>
-      </c>
-      <c r="G49" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="G49" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="H49" s="30" t="s">
+      <c r="H49" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="21" t="s">
+    <row r="50" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="22" t="s">
+      <c r="C50" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="18" t="s">
         <v>182</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F50" s="23" t="s">
-        <v>296</v>
-      </c>
-      <c r="G50" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="G50" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="H50" s="30" t="s">
+      <c r="H50" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I50" s="22" t="s">
+      <c r="I50" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J50" s="25"/>
+      <c r="J50" s="19"/>
     </row>
     <row r="51" spans="1:15" s="12" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
@@ -3429,22 +3356,22 @@
         <v>184</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F51" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="G51" s="18" t="s">
+      <c r="G51" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H51" s="18" t="s">
+      <c r="H51" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I51" s="12" t="s">
         <v>23</v>
       </c>
       <c r="J51" s="13"/>
-      <c r="M51" s="16" t="s">
+      <c r="M51" s="23" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3462,15 +3389,15 @@
         <v>187</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G52" s="18" t="s">
+      <c r="G52" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H52" s="18" t="s">
+      <c r="H52" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I52" s="12" t="s">
@@ -3491,194 +3418,194 @@
         <v>189</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="G53" s="18" t="s">
+      <c r="G53" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="H53" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="21" t="s">
+    <row r="54" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="B54" s="22" t="s">
+      <c r="B54" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="C54" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="22" t="s">
+      <c r="C54" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="18" t="s">
         <v>198</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F54" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="F54" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="G54" s="24" t="s">
+      <c r="G54" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H54" s="18" t="s">
+      <c r="H54" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="I54" s="22" t="s">
+      <c r="I54" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="J54" s="25"/>
-    </row>
-    <row r="55" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="21" t="s">
+      <c r="J54" s="19"/>
+    </row>
+    <row r="55" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="22" t="s">
+      <c r="C55" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="18" t="s">
         <v>201</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F55" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="F55" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="G55" s="24" t="s">
+      <c r="G55" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H55" s="18" t="s">
+      <c r="H55" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="I55" s="22" t="s">
+      <c r="I55" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="J55" s="25"/>
-    </row>
-    <row r="56" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="21" t="s">
+      <c r="J55" s="19"/>
+    </row>
+    <row r="56" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="C56" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="22" t="s">
+      <c r="C56" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="18" t="s">
         <v>203</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F56" t="s">
+        <v>280</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="G56" s="22" t="s">
+      <c r="G56" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H56" s="30" t="s">
+      <c r="H56" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I56" s="26" t="s">
+      <c r="I56" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="J56" s="25"/>
-    </row>
-    <row r="57" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="21" t="s">
+      <c r="J56" s="19"/>
+    </row>
+    <row r="57" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="C57" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="22" t="s">
+      <c r="C57" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="18" t="s">
         <v>207</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F57" t="s">
-        <v>297</v>
-      </c>
-      <c r="G57" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="G57" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H57" s="30" t="s">
+      <c r="H57" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I57" s="22" t="s">
+      <c r="I57" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J57" s="25"/>
-    </row>
-    <row r="58" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="21" t="s">
+      <c r="J57" s="19"/>
+    </row>
+    <row r="58" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="C58" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="22" t="s">
+      <c r="C58" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="18" t="s">
         <v>209</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F58" t="s">
-        <v>298</v>
-      </c>
-      <c r="G58" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="G58" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H58" s="30" t="s">
+      <c r="H58" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I58" s="22" t="s">
+      <c r="I58" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="J58" s="25"/>
+      <c r="J58" s="19"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="17" t="s">
         <v>230</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="22" t="s">
+      <c r="C59" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="18" t="s">
         <v>232</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F59" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G59" s="22" t="s">
+      <c r="G59" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H59" s="30" t="s">
+      <c r="H59" s="10" t="s">
         <v>274</v>
       </c>
       <c r="N59" s="4" t="s">
@@ -3686,28 +3613,28 @@
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="17" t="s">
         <v>234</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C60" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="22" t="s">
+      <c r="C60" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="18" t="s">
         <v>236</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="G60" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="G60" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H60" s="30" t="s">
+      <c r="H60" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I60" s="4" t="s">
@@ -3721,28 +3648,28 @@
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="17" t="s">
         <v>239</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C61" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="22" t="s">
+      <c r="C61" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="18" t="s">
         <v>241</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="G61" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="G61" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H61" s="30" t="s">
+      <c r="H61" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I61" s="4" t="s">
@@ -3753,28 +3680,28 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A62" s="21" t="s">
+      <c r="A62" s="17" t="s">
         <v>253</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>248</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F62" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G62" s="18" t="s">
+      <c r="G62" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H62" s="18" t="s">
+      <c r="H62" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I62" s="4" t="s">
@@ -3788,60 +3715,60 @@
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A63" s="21" t="s">
+      <c r="A63" s="17" t="s">
         <v>254</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C63" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>250</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F63" t="s">
+        <v>280</v>
+      </c>
+      <c r="F63" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G63" s="18" t="s">
+      <c r="G63" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H63" s="18" t="s">
+      <c r="H63" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="N63" s="28" t="s">
+      <c r="N63" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="O63" s="1" t="s">
+      <c r="O63" s="4" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A64" s="21" t="s">
+      <c r="A64" s="17" t="s">
         <v>255</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F64" t="s">
+        <v>280</v>
+      </c>
+      <c r="F64" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G64" s="18" t="s">
+      <c r="G64" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H64" s="18" t="s">
+      <c r="H64" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I64" s="4" t="s">
@@ -3852,28 +3779,28 @@
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="17" t="s">
         <v>256</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C65" s="22" t="s">
+      <c r="C65" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>249</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F65" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F65" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G65" s="18" t="s">
+      <c r="G65" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H65" s="18" t="s">
+      <c r="H65" s="20" t="s">
         <v>219</v>
       </c>
       <c r="I65" s="4" t="s">
@@ -3887,118 +3814,118 @@
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A66" s="21" t="s">
+      <c r="A66" s="17" t="s">
         <v>262</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C66" s="22" t="s">
+      <c r="C66" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>264</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F66" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F66" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G66" s="22" t="s">
+      <c r="G66" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H66" s="30" t="s">
+      <c r="H66" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I66" s="22" t="s">
+      <c r="I66" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A67" s="21" t="s">
+      <c r="A67" s="17" t="s">
         <v>265</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="C67" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>267</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F67" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F67" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G67" s="22" t="s">
+      <c r="G67" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H67" s="30" t="s">
+      <c r="H67" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I67" s="22" t="s">
+      <c r="I67" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A68" s="21" t="s">
+      <c r="A68" s="17" t="s">
         <v>268</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="C68" s="22" t="s">
+      <c r="C68" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>270</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="G68" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G68" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H68" s="30" t="s">
+      <c r="H68" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I68" s="22" t="s">
+      <c r="I68" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A69" s="21" t="s">
+      <c r="A69" s="17" t="s">
         <v>271</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="C69" s="22" t="s">
+      <c r="C69" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>273</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="G69" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G69" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H69" s="30" t="s">
+      <c r="H69" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="I69" s="22" t="s">
+      <c r="I69" s="18" t="s">
         <v>23</v>
       </c>
       <c r="N69" s="4" t="s">
@@ -4006,82 +3933,98 @@
       </c>
     </row>
     <row r="70" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A70" s="21" t="s">
+      <c r="A70" s="17" t="s">
         <v>261</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C70" s="22" t="s">
+      <c r="C70" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>260</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F70" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G70" s="18" t="s">
+      <c r="G70" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H70" s="18" t="s">
+      <c r="H70" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="I70" s="22" t="s">
+      <c r="I70" s="18" t="s">
         <v>115</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>259</v>
       </c>
     </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A71" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G71" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="I71" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A72" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G72" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="I72" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M70" xr:uid="{EB08446A-0716-488E-B42E-00D2DA842126}"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="G17" r:id="rId1" xr:uid="{723970F4-4603-469C-B45C-96036D0B804A}"/>
-    <hyperlink ref="H17" r:id="rId2" xr:uid="{2AD4D63B-2996-4EF0-8A2F-8AF5B6BD9CC8}"/>
-    <hyperlink ref="G18:G33" r:id="rId3" display="rashmi.rl@thomsonreuters.com" xr:uid="{3DB5E2C0-A750-4358-9BF6-32D3D98D2096}"/>
-    <hyperlink ref="G33" r:id="rId4" xr:uid="{17A7C8C6-2597-4D73-A91A-12BAC045FE55}"/>
-    <hyperlink ref="G34" r:id="rId5" xr:uid="{5B70CB00-7AFC-441C-8B21-F20FFAC5C9AF}"/>
-    <hyperlink ref="G35" r:id="rId6" xr:uid="{52261ED4-7225-4B8F-970A-9E1807022FE1}"/>
-    <hyperlink ref="G36" r:id="rId7" xr:uid="{501C3C63-1543-43E6-8460-64278CEC18A9}"/>
-    <hyperlink ref="G37" r:id="rId8" xr:uid="{CDA235E6-241E-4DCC-ACAE-541EAE638029}"/>
-    <hyperlink ref="G38" r:id="rId9" xr:uid="{2CC833FE-2CFA-4F55-A03C-0F6D36B8FF1A}"/>
-    <hyperlink ref="G39" r:id="rId10" xr:uid="{7CB5209A-D384-479E-ABBE-818E4A32E00E}"/>
-    <hyperlink ref="G40" r:id="rId11" xr:uid="{8398B387-7BC7-498B-9AA4-042A87D3A4DB}"/>
-    <hyperlink ref="G41" r:id="rId12" xr:uid="{F030BE8B-BC36-49E1-8D71-1478C5C4BCDF}"/>
-    <hyperlink ref="G42" r:id="rId13" xr:uid="{23135E44-8E96-4D83-A082-A7511C1C0771}"/>
-    <hyperlink ref="G43" r:id="rId14" xr:uid="{0CCCEC04-DDD0-4D0F-8D23-C47F6F6CEC53}"/>
-    <hyperlink ref="G44" r:id="rId15" xr:uid="{D466216C-1EF1-4553-A660-7BF606C27DB9}"/>
-    <hyperlink ref="G45" r:id="rId16" xr:uid="{F86289C3-3FA2-4BA4-AEDD-552CD06D34E6}"/>
-    <hyperlink ref="G46" r:id="rId17" xr:uid="{0DE6A34B-2C8E-4613-99BD-7169693A3191}"/>
-    <hyperlink ref="G47" r:id="rId18" xr:uid="{0E6F7DF1-DD17-41D2-B68A-807CE6F4A387}"/>
-    <hyperlink ref="G48" r:id="rId19" xr:uid="{111B4475-977A-49B9-9657-CCB615DEF79F}"/>
-    <hyperlink ref="G49" r:id="rId20" xr:uid="{471A5D33-835A-414E-97B8-362512B11F19}"/>
-    <hyperlink ref="G50" r:id="rId21" xr:uid="{C7E5B850-A6A3-47EB-B6C2-A656ABE578C3}"/>
-    <hyperlink ref="H46" r:id="rId22" xr:uid="{4A959DA8-94AE-478F-AA59-3FF5B726B06D}"/>
-    <hyperlink ref="G51" r:id="rId23" xr:uid="{4930390E-877B-48E6-806D-25B7F1D8C5B8}"/>
-    <hyperlink ref="G52" r:id="rId24" xr:uid="{F7B5D713-A9B5-4133-BD07-98197D7E72D4}"/>
-    <hyperlink ref="G53" r:id="rId25" xr:uid="{E5AB4738-A96D-4977-A386-A581CA3C01E6}"/>
-    <hyperlink ref="G54" r:id="rId26" xr:uid="{DE1E9284-2F49-42F1-A7C3-B0CEC31B6EFD}"/>
-    <hyperlink ref="G55" r:id="rId27" xr:uid="{E2B9685A-2447-4FE1-AF1B-C87EA1440D7B}"/>
-    <hyperlink ref="H18:H42" r:id="rId28" display="Test@123" xr:uid="{428C5C26-7283-4267-926D-F8A15A909940}"/>
-    <hyperlink ref="H51:H55" r:id="rId29" display="Test@123" xr:uid="{1F19B917-4AC7-4318-9D2C-B3B3447CBA4E}"/>
-    <hyperlink ref="G62" r:id="rId30" xr:uid="{C837631E-D83F-4CAB-B7EF-359AC0B72C2C}"/>
-    <hyperlink ref="G63" r:id="rId31" xr:uid="{B216E578-99F7-4539-95BC-CEAE985CF4A1}"/>
-    <hyperlink ref="G64" r:id="rId32" xr:uid="{1E1ADCC4-95BC-4AF8-9AB3-7EE388B85F1D}"/>
-    <hyperlink ref="G65" r:id="rId33" xr:uid="{C0E8DCD0-B5EB-40AA-B3E2-20F3244F6E65}"/>
-    <hyperlink ref="H62" r:id="rId34" xr:uid="{111BCB90-F2D5-450B-B749-7249F56DBF39}"/>
-    <hyperlink ref="H63" r:id="rId35" xr:uid="{29167A98-D6C2-4F18-BA83-7020E938AB86}"/>
-    <hyperlink ref="H64" r:id="rId36" xr:uid="{B0A91A7F-96A4-477C-9A31-4C51B69E3C70}"/>
-    <hyperlink ref="H65" r:id="rId37" xr:uid="{6DA28F36-CB17-4142-B2C8-A1F53BE08003}"/>
-    <hyperlink ref="G70" r:id="rId38" xr:uid="{6303DB8D-1B7E-4608-812E-AB683479C51C}"/>
-    <hyperlink ref="H70" r:id="rId39" xr:uid="{3EC9ABF3-377B-46E8-8585-FD35C630B6C3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId40"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the test scripts issues
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3B95AC-DC94-4379-AFA1-E8843A499793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0F4DAD-1CD4-4A5C-A43A-61BAE9C4294A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Module" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="282">
   <si>
     <t>TSID</t>
   </si>
@@ -719,9 +719,6 @@
     <t xml:space="preserve">polyethylene </t>
   </si>
   <si>
-    <t>resin</t>
-  </si>
-  <si>
     <t>CHEMEXP-1086</t>
   </si>
   <si>
@@ -1038,6 +1035,57 @@
   </si>
   <si>
     <t xml:space="preserve">CHEMEXP-1824 </t>
+  </si>
+  <si>
+    <t>anand.perumallukamichetty@clarivate.com</t>
+  </si>
+  <si>
+    <t>Fail:clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-dcq-c166="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="cdx secondary disabled button" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg mat-stroked-button mat-button-base mat-primary" title="company/organization" style="margin-right: 2px; place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1155, 405). Other element would receive the click: &lt;p _ngcontent-dcq-c162=""&gt;...&lt;/p&gt;
+  (Session info: chrome=97.0.4692.71)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.71, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56994}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 8662336e9619b3137767269c7ec9a033clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-dcq-c166="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="cdx secondary disabled button" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg mat-stroked-button mat-button-base mat-primary" title="company/organization" style="margin-right: 2px; place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1155, 405). Other element would receive the click: &lt;p _ngcontent-dcq-c162=""&gt;...&lt;/p&gt;
+  (Session info: chrome=97.0.4692.71)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.71, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56994}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 8662336e9619b3137767269c7ec9a033</t>
+  </si>
+  <si>
+    <t>Fail:clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-wok-c171="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="icon" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg cdx-but-link org mat-stroked-button mat-button-base mat-primary" title="company/organization" style="place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1457, 189). Other element would receive the click: &lt;p _ngcontent-wok-c162=""&gt;...&lt;/p&gt;
+  (Session info: chrome=97.0.4692.71)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.71, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57357}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 472697228d15dfb703788ae9d7b9ab29clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-wok-c171="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="icon" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg cdx-but-link org mat-stroked-button mat-button-base mat-primary" title="company/organization" style="place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1457, 189). Other element would receive the click: &lt;p _ngcontent-wok-c162=""&gt;...&lt;/p&gt;
+  (Session info: chrome=97.0.4692.71)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.71, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57357}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 472697228d15dfb703788ae9d7b9ab29</t>
+  </si>
+  <si>
+    <t>Derwent@2022</t>
+  </si>
+  <si>
+    <t>Fail:clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-mqw-c166="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="cdx secondary disabled button" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg mat-stroked-button mat-button-base mat-primary" title="company/organization" style="margin-right: 2px; place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1462, 513). Other element would receive the click: &lt;p _ngcontent-mqw-c162=""&gt;...&lt;/p&gt;
+  (Session info: chrome=97.0.4692.99)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.99, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60597}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 34b59cc70165802c31f01acc28bca7ccclickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-mqw-c166="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="cdx secondary disabled button" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg mat-stroked-button mat-button-base mat-primary" title="company/organization" style="margin-right: 2px; place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1462, 513). Other element would receive the click: &lt;p _ngcontent-mqw-c162=""&gt;...&lt;/p&gt;
+  (Session info: chrome=97.0.4692.99)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.99, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60597}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 34b59cc70165802c31f01acc28bca7cc</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1192,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1157,6 +1205,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1504,17 +1553,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.109375" style="1" collapsed="1"/>
+    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1546,32 +1595,32 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="69.33203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="54.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.5546875" style="3" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="69.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="54.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.5703125" style="3" hidden="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="255" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.33203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.33203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="70.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="70.42578125" style="3" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="40" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.6640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.33203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.88671875" style="3" collapsed="1"/>
+    <col min="12" max="12" width="203.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="132.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.85546875" style="3" collapsed="1"/>
     <col min="15" max="15" width="28" style="3" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="27.44140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="16384" width="8.88671875" style="3" collapsed="1"/>
+    <col min="16" max="16" width="27.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="16384" width="8.85546875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1613,13 +1662,13 @@
         <v>196</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>82</v>
       </c>
@@ -1633,22 +1682,22 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>267</v>
+      <c r="H2" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>83</v>
       </c>
@@ -1662,22 +1711,22 @@
         <v>19</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>267</v>
+      <c r="H3" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>84</v>
       </c>
@@ -1691,22 +1740,22 @@
         <v>22</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>267</v>
+      <c r="H4" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>85</v>
       </c>
@@ -1720,22 +1769,22 @@
         <v>26</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>267</v>
+      <c r="H5" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>86</v>
       </c>
@@ -1749,22 +1798,22 @@
         <v>28</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>267</v>
+      <c r="H6" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>87</v>
       </c>
@@ -1778,16 +1827,16 @@
         <v>30</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>267</v>
+      <c r="H7" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>31</v>
@@ -1796,7 +1845,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>88</v>
       </c>
@@ -1810,16 +1859,16 @@
         <v>34</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>267</v>
+      <c r="H8" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>35</v>
@@ -1828,7 +1877,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>89</v>
       </c>
@@ -1842,16 +1891,16 @@
         <v>37</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>267</v>
+      <c r="H9" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>35</v>
@@ -1860,7 +1909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>90</v>
       </c>
@@ -1874,22 +1923,22 @@
         <v>40</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>267</v>
+      <c r="H10" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>91</v>
       </c>
@@ -1903,16 +1952,16 @@
         <v>43</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>267</v>
+      <c r="H11" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>20</v>
@@ -1921,7 +1970,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>92</v>
       </c>
@@ -1935,16 +1984,16 @@
         <v>45</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>267</v>
+      <c r="H12" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>20</v>
@@ -1953,7 +2002,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>94</v>
       </c>
@@ -1967,16 +2016,16 @@
         <v>47</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>267</v>
+      <c r="H13" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>20</v>
@@ -1985,7 +2034,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>95</v>
       </c>
@@ -1999,16 +2048,16 @@
         <v>50</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>267</v>
+      <c r="H14" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>20</v>
@@ -2017,7 +2066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>96</v>
       </c>
@@ -2031,16 +2080,16 @@
         <v>52</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>267</v>
+      <c r="H15" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>35</v>
@@ -2049,7 +2098,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>97</v>
       </c>
@@ -2063,22 +2112,22 @@
         <v>61</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>267</v>
+      <c r="H16" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>98</v>
       </c>
@@ -2092,22 +2141,22 @@
         <v>62</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>267</v>
+      <c r="H17" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>99</v>
       </c>
@@ -2121,22 +2170,22 @@
         <v>67</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>267</v>
+      <c r="H18" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>100</v>
       </c>
@@ -2150,22 +2199,22 @@
         <v>64</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>267</v>
+      <c r="H19" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>101</v>
       </c>
@@ -2179,22 +2228,22 @@
         <v>77</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>267</v>
+      <c r="H20" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>102</v>
       </c>
@@ -2208,19 +2257,19 @@
         <v>69</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>267</v>
+      <c r="H21" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>103</v>
+        <v>20</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>70</v>
@@ -2229,12 +2278,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
@@ -2243,22 +2292,22 @@
         <v>75</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>267</v>
+        <v>273</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>107</v>
       </c>
@@ -2272,22 +2321,22 @@
         <v>56</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>267</v>
+      <c r="H23" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>108</v>
       </c>
@@ -2301,19 +2350,19 @@
         <v>58</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>109</v>
       </c>
@@ -2327,22 +2376,22 @@
         <v>60</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>267</v>
+      <c r="H25" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>110</v>
       </c>
@@ -2356,22 +2405,22 @@
         <v>79</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>267</v>
+      <c r="H26" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>111</v>
       </c>
@@ -2385,16 +2434,16 @@
         <v>72</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>267</v>
+      <c r="H27" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>73</v>
@@ -2403,7 +2452,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>113</v>
       </c>
@@ -2417,22 +2466,22 @@
         <v>112</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>267</v>
+      <c r="H28" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>116</v>
       </c>
@@ -2446,22 +2495,22 @@
         <v>118</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>267</v>
+      <c r="H29" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>119</v>
       </c>
@@ -2475,22 +2524,22 @@
         <v>121</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>267</v>
+      <c r="H30" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>122</v>
       </c>
@@ -2504,22 +2553,22 @@
         <v>124</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>267</v>
+      <c r="H31" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>125</v>
       </c>
@@ -2533,22 +2582,22 @@
         <v>126</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>267</v>
+      <c r="H32" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>127</v>
       </c>
@@ -2562,23 +2611,23 @@
         <v>129</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="5" t="s">
         <v>176</v>
       </c>
       <c r="H33" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I33" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="5" customFormat="1" ht="99.9" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" s="5" customFormat="1" ht="99.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>130</v>
       </c>
@@ -2592,23 +2641,23 @@
         <v>132</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="5" t="s">
         <v>176</v>
       </c>
       <c r="H34" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I34" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>133</v>
       </c>
@@ -2622,23 +2671,23 @@
         <v>134</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H35" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I35" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>135</v>
       </c>
@@ -2652,23 +2701,23 @@
         <v>136</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H36" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I36" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>137</v>
       </c>
@@ -2682,22 +2731,22 @@
         <v>139</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>267</v>
+      <c r="H37" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>140</v>
       </c>
@@ -2711,22 +2760,22 @@
         <v>142</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>267</v>
+      <c r="H38" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="5" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="5" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>143</v>
       </c>
@@ -2740,23 +2789,23 @@
         <v>145</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H39" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I39" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J39" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="5" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" s="5" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>146</v>
       </c>
@@ -2770,23 +2819,23 @@
         <v>148</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H40" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I40" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>149</v>
       </c>
@@ -2800,22 +2849,22 @@
         <v>151</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>267</v>
+      <c r="H41" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="5" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" s="5" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>152</v>
       </c>
@@ -2829,23 +2878,23 @@
         <v>154</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H42" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I42" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>167</v>
       </c>
@@ -2859,22 +2908,22 @@
         <v>156</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>267</v>
+      <c r="H43" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>168</v>
       </c>
@@ -2888,22 +2937,22 @@
         <v>159</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>267</v>
+      <c r="H44" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>169</v>
       </c>
@@ -2917,23 +2966,23 @@
         <v>161</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H45" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I45" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>170</v>
       </c>
@@ -2947,22 +2996,22 @@
         <v>162</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H46" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>267</v>
+      <c r="H46" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>171</v>
       </c>
@@ -2976,22 +3025,22 @@
         <v>164</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H47" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>267</v>
+      <c r="H47" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>172</v>
       </c>
@@ -3005,22 +3054,22 @@
         <v>166</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H48" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>267</v>
+      <c r="H48" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>191</v>
       </c>
@@ -3034,22 +3083,22 @@
         <v>179</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H49" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>267</v>
+      <c r="H49" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>192</v>
       </c>
@@ -3063,23 +3112,23 @@
         <v>182</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H50" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I50" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="5" customFormat="1" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" s="5" customFormat="1" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>193</v>
       </c>
@@ -3093,17 +3142,17 @@
         <v>184</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H51" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I51" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>23</v>
@@ -3112,7 +3161,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>194</v>
       </c>
@@ -3126,22 +3175,22 @@
         <v>187</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H52" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>267</v>
+      <c r="H52" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>195</v>
       </c>
@@ -3155,24 +3204,24 @@
         <v>189</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H53" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>267</v>
+      <c r="H53" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>197</v>
@@ -3184,24 +3233,24 @@
         <v>198</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H54" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>267</v>
+      <c r="H54" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>199</v>
@@ -3213,22 +3262,22 @@
         <v>200</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H55" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>267</v>
+      <c r="H55" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>207</v>
       </c>
@@ -3242,22 +3291,22 @@
         <v>202</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H56" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>267</v>
+      <c r="H56" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>208</v>
       </c>
@@ -3271,22 +3320,22 @@
         <v>204</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H57" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>267</v>
+      <c r="H57" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>209</v>
       </c>
@@ -3300,476 +3349,476 @@
         <v>206</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H58" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>267</v>
+      <c r="H58" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="3" t="s">
+      <c r="E59" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="O59" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="O59" s="3" t="s">
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>223</v>
-      </c>
       <c r="E60" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H60" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>267</v>
+      <c r="H60" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K60" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="O60" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="O60" s="3" t="s">
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="3" t="s">
+      <c r="E61" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="J61" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E61" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="J61" s="3" t="s">
+      <c r="O61" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="O61" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>230</v>
-      </c>
       <c r="C62" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H62" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>267</v>
+      <c r="H62" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K62" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="O62" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="O62" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="O63" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="P63" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="3" t="s">
+      <c r="B64" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E63" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="O63" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="P63" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>238</v>
-      </c>
       <c r="E64" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H64" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>267</v>
+      <c r="H64" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>20</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H65" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>267</v>
+      <c r="H65" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J65" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K65" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="O65" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="O65" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="C66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>250</v>
-      </c>
       <c r="E66" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H66" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>267</v>
+      <c r="H66" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J66" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="C67" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>253</v>
-      </c>
       <c r="E67" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H67" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I67" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="J67" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C68" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>267</v>
+        <v>281</v>
+      </c>
+      <c r="H68" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>259</v>
-      </c>
       <c r="E69" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>267</v>
+        <v>278</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>23</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I70" s="3" t="s">
-        <v>267</v>
+        <v>279</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J70" s="3" t="s">
         <v>115</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>261</v>
-      </c>
       <c r="E71" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H71" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>267</v>
+      <c r="H71" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J71" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B72" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>263</v>
-      </c>
       <c r="E72" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H72" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>267</v>
+      <c r="H72" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J72" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B73" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="C73" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>276</v>
-      </c>
       <c r="E73" s="7" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>176</v>
@@ -3777,11 +3826,11 @@
       <c r="G73" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="H73" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="I73" s="7" t="s">
-        <v>267</v>
+      <c r="H73" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J73" s="7" t="s">
         <v>20</v>
@@ -3795,6 +3844,7 @@
   <autoFilter ref="A1:P73" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
     <filterColumn colId="4">
       <filters>
+        <filter val="Rerun"/>
         <filter val="Y"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
fixed Automation regression issues and and added december scoped automation scripts CHEMEXP-1982 CHEMEXP-1983 CHEMEXP-1984 CHEMEXP-1985
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0F4DAD-1CD4-4A5C-A43A-61BAE9C4294A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE113EC-5475-4998-A0FC-0157AF1986D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Module" sheetId="2" r:id="rId1"/>
     <sheet name="chemicalsearch" sheetId="80" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">chemicalsearch!$A$1:$P$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">chemicalsearch!$A$1:$P$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="294">
   <si>
     <t>TSID</t>
   </si>
@@ -1040,52 +1040,52 @@
     <t>anand.perumallukamichetty@clarivate.com</t>
   </si>
   <si>
-    <t>Fail:clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-dcq-c166="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="cdx secondary disabled button" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg mat-stroked-button mat-button-base mat-primary" title="company/organization" style="margin-right: 2px; place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1155, 405). Other element would receive the click: &lt;p _ngcontent-dcq-c162=""&gt;...&lt;/p&gt;
-  (Session info: chrome=97.0.4692.71)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.71, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56994}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 8662336e9619b3137767269c7ec9a033clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-dcq-c166="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="cdx secondary disabled button" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg mat-stroked-button mat-button-base mat-primary" title="company/organization" style="margin-right: 2px; place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1155, 405). Other element would receive the click: &lt;p _ngcontent-dcq-c162=""&gt;...&lt;/p&gt;
-  (Session info: chrome=97.0.4692.71)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.71, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:56994}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 8662336e9619b3137767269c7ec9a033</t>
-  </si>
-  <si>
-    <t>Fail:clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-wok-c171="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="icon" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg cdx-but-link org mat-stroked-button mat-button-base mat-primary" title="company/organization" style="place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1457, 189). Other element would receive the click: &lt;p _ngcontent-wok-c162=""&gt;...&lt;/p&gt;
-  (Session info: chrome=97.0.4692.71)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.71, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57357}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 472697228d15dfb703788ae9d7b9ab29clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-wok-c171="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="icon" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg cdx-but-link org mat-stroked-button mat-button-base mat-primary" title="company/organization" style="place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1457, 189). Other element would receive the click: &lt;p _ngcontent-wok-c162=""&gt;...&lt;/p&gt;
-  (Session info: chrome=97.0.4692.71)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.71, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57357}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 472697228d15dfb703788ae9d7b9ab29</t>
-  </si>
-  <si>
     <t>Derwent@2022</t>
   </si>
   <si>
-    <t>Fail:clickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-mqw-c166="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="cdx secondary disabled button" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg mat-stroked-button mat-button-base mat-primary" title="company/organization" style="margin-right: 2px; place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1462, 513). Other element would receive the click: &lt;p _ngcontent-mqw-c162=""&gt;...&lt;/p&gt;
-  (Session info: chrome=97.0.4692.99)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.99, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60597}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 34b59cc70165802c31f01acc28bca7ccclickOnOrganizationIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;button _ngcontent-mqw-c166="" aria-haspopup="true" type="button" mat-stroked-button="" color="primary" aria-label="cdx secondary disabled button" fxlayoutalign="center center" class="mat-focus-indicator mat-menu-trigger cdx-but-lg mat-stroked-button mat-button-base mat-primary" title="company/organization" style="margin-right: 2px; place-content: center; align-items: center; flex-direction: row; box-sizing: border-box; display: flex;"&gt;...&lt;/button&gt; is not clickable at point (1462, 513). Other element would receive the click: &lt;p _ngcontent-mqw-c162=""&gt;...&lt;/p&gt;
-  (Session info: chrome=97.0.4692.99)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 97.0.4692.99, chrome: {chromedriverVersion: 97.0.4692.71 (adefa7837d02a..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60597}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 34b59cc70165802c31f01acc28bca7cc</t>
+    <t>Validate PDF links in the Patent Record View</t>
+  </si>
+  <si>
+    <t>vaildatePDFPatentRecordView</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate RS sort options </t>
+  </si>
+  <si>
+    <t>vaildateRsSortOptions</t>
+  </si>
+  <si>
+    <t>Validate chemical role filter</t>
+  </si>
+  <si>
+    <t>vaildateChemicalRoleFilterOptions</t>
+  </si>
+  <si>
+    <t>Validate search History functionality</t>
+  </si>
+  <si>
+    <t>validateSearchistoryFuntionality</t>
+  </si>
+  <si>
+    <t>azobisisobutyronitrile</t>
+  </si>
+  <si>
+    <t>initiator radical</t>
+  </si>
+  <si>
+    <t>azobis</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1982</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1983</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1984</t>
+  </si>
+  <si>
+    <t>CHEMEXP-1985</t>
   </si>
 </sst>
 </file>
@@ -1192,20 +1192,19 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1556,14 +1555,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" width="25.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1593,34 +1592,34 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="69.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="54.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="255" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="70.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="40" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="203.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="132.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.85546875" style="3" collapsed="1"/>
-    <col min="15" max="15" width="28" style="3" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="27.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="16384" width="8.85546875" style="3" collapsed="1"/>
+    <col min="1" max="1" width="25.6640625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="69.33203125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="54.6640625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.5546875" style="3" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="255" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.33203125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.33203125" style="6" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="70.44140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="40" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="203.33203125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="132.109375" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.88671875" style="6" collapsed="1"/>
+    <col min="15" max="15" width="28" style="6" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="27.44140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="16384" width="8.88671875" style="6" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1668,936 +1667,936 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="E4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="E5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="E6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="E7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="E8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="6" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J9" s="3" t="s">
+      <c r="E9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J10" s="3" t="s">
+      <c r="E10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="E11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J12" s="3" t="s">
+      <c r="E12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="E13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J14" s="3" t="s">
+      <c r="E14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="C15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J15" s="3" t="s">
+      <c r="E15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="E16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="C17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J17" s="3" t="s">
+      <c r="E17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J17" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="C18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J18" s="3" t="s">
+      <c r="E18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J18" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="C19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J19" s="3" t="s">
+      <c r="E19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="C20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J20" s="3" t="s">
+      <c r="E20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="C21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J21" s="3" t="s">
+      <c r="E21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="M21" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="C22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J22" s="3" t="s">
+      <c r="E22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J22" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J23" s="3" t="s">
+      <c r="E23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="C24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="E24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="C25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J25" s="3" t="s">
+      <c r="E25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J26" s="3" t="s">
+      <c r="E26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J26" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="C27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J27" s="3" t="s">
+      <c r="E27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J27" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="C28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J28" s="3" t="s">
+      <c r="E28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J28" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="C29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J29" s="3" t="s">
+      <c r="E29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="C30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J30" s="3" t="s">
+      <c r="E30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J30" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="C31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J31" s="3" t="s">
+      <c r="E31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J31" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="C32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J32" s="3" t="s">
+      <c r="E32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J32" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>127</v>
       </c>
@@ -2610,7 +2609,7 @@
       <c r="D33" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F33" s="3"/>
@@ -2627,7 +2626,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="5" customFormat="1" ht="99.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="5" customFormat="1" ht="99.9" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>130</v>
       </c>
@@ -2640,7 +2639,7 @@
       <c r="D34" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F34" s="3"/>
@@ -2657,7 +2656,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>133</v>
       </c>
@@ -2670,7 +2669,7 @@
       <c r="D35" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F35" s="3"/>
@@ -2687,7 +2686,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>135</v>
       </c>
@@ -2700,7 +2699,7 @@
       <c r="D36" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F36" s="3"/>
@@ -2717,65 +2716,65 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="3" t="s">
+      <c r="C37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J37" s="3" t="s">
+      <c r="E37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J37" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="C38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J38" s="3" t="s">
+      <c r="E38" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J38" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="5" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="5" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>143</v>
       </c>
@@ -2788,7 +2787,7 @@
       <c r="D39" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F39" s="3"/>
@@ -2805,7 +2804,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="5" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="5" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>146</v>
       </c>
@@ -2818,7 +2817,7 @@
       <c r="D40" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F40" s="3"/>
@@ -2835,36 +2834,36 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="C41" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J41" s="3" t="s">
+      <c r="E41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J41" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="5" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="5" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>152</v>
       </c>
@@ -2877,7 +2876,7 @@
       <c r="D42" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F42" s="3"/>
@@ -2894,65 +2893,65 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="3" t="s">
+      <c r="C43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J43" s="3" t="s">
+      <c r="E43" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J43" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="3" t="s">
+      <c r="C44" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J44" s="3" t="s">
+      <c r="E44" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J44" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>169</v>
       </c>
@@ -2965,7 +2964,7 @@
       <c r="D45" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F45" s="3"/>
@@ -2982,123 +2981,123 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="3" t="s">
+      <c r="C46" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E46" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J46" s="3" t="s">
+      <c r="E46" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J46" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="3" t="s">
+      <c r="C47" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J47" s="3" t="s">
+      <c r="E47" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="3" t="s">
+      <c r="C48" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="E48" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J48" s="3" t="s">
+      <c r="E48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J48" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="3" t="s">
+      <c r="C49" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J49" s="3" t="s">
+      <c r="E49" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>192</v>
       </c>
@@ -3111,7 +3110,7 @@
       <c r="D50" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E50" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F50" s="3"/>
@@ -3128,7 +3127,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="5" customFormat="1" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="5" customFormat="1" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>193</v>
       </c>
@@ -3141,7 +3140,7 @@
       <c r="D51" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F51" s="3"/>
@@ -3161,469 +3160,469 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="3" t="s">
+      <c r="C52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E52" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H52" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J52" s="3" t="s">
+      <c r="E52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J52" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="3" t="s">
+      <c r="C53" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E53" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I53" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J53" s="3" t="s">
+      <c r="E53" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J53" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="3" t="s">
+      <c r="C54" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E54" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I54" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J54" s="3" t="s">
+      <c r="E54" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J54" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="3" t="s">
+      <c r="C55" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E55" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I55" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J55" s="3" t="s">
+      <c r="E55" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J55" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="3" t="s">
+      <c r="C56" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H56" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I56" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J56" s="3" t="s">
+      <c r="E56" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J56" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="3" t="s">
+      <c r="C57" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="E57" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H57" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I57" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J57" s="3" t="s">
+      <c r="E57" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="3" t="s">
+      <c r="C58" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I58" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J58" s="3" t="s">
+      <c r="E58" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J58" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="3" t="s">
+      <c r="C59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H59" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I59" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="O59" s="3" t="s">
+      <c r="E59" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="O59" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="3" t="s">
+      <c r="C60" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="E60" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H60" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I60" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J60" s="3" t="s">
+      <c r="E60" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J60" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K60" s="3" t="s">
+      <c r="K60" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="O60" s="3" t="s">
+      <c r="O60" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="3" t="s">
+      <c r="C61" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="E61" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H61" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I61" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J61" s="3" t="s">
+      <c r="E61" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J61" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="O61" s="3" t="s">
+      <c r="O61" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D62" s="3" t="s">
+      <c r="C62" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E62" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H62" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I62" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J62" s="3" t="s">
+      <c r="E62" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J62" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K62" s="3" t="s">
+      <c r="K62" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="O62" s="3" t="s">
+      <c r="O62" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="3" t="s">
+      <c r="C63" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="E63" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H63" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I63" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="O63" s="3" t="s">
+      <c r="E63" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="O63" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="P63" s="3" t="s">
+      <c r="P63" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="3" t="s">
+      <c r="C64" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E64" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H64" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I64" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J64" s="3" t="s">
+      <c r="E64" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J64" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="O64" s="3" t="s">
+      <c r="O64" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" s="3" t="s">
+      <c r="C65" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E65" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H65" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I65" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J65" s="3" t="s">
+      <c r="E65" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J65" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K65" s="3" t="s">
+      <c r="K65" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="O65" s="3" t="s">
+      <c r="O65" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D66" s="3" t="s">
+      <c r="C66" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E66" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H66" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I66" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J66" s="3" t="s">
+      <c r="E66" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J66" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>250</v>
       </c>
@@ -3636,7 +3635,7 @@
       <c r="D67" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="6" t="s">
         <v>273</v>
       </c>
       <c r="F67" s="3"/>
@@ -3653,198 +3652,315 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="3" t="s">
+      <c r="C68" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="E68" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G68" s="3" t="s">
+      <c r="E68" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O69" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I70" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K70" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A71" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I71" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A72" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I72" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I74" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="H68" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I68" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J68" s="3" t="s">
+      <c r="C75" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I75" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J75" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="H69" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I69" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O69" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="H70" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I70" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H71" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I71" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H72" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I72" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="G73" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="H73" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I73" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J73" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
-      <c r="M73" s="6"/>
-      <c r="N73" s="6"/>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I76" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I77" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O77" s="6" t="s">
+        <v>287</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P73" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
+  <autoFilter ref="A1:P77" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
     <filterColumn colId="4">
       <filters>
-        <filter val="Rerun"/>
         <filter val="Y"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
fixed jenkins issues and commented out the literature code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF49A917-DB77-4065-AC15-4B8B1109FB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D5B125-7501-4DCF-BF5C-C2A64F8970E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Module" sheetId="2" r:id="rId1"/>
     <sheet name="chemicalsearch" sheetId="80" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">chemicalsearch!$A$1:$P$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">chemicalsearch!$A$1:$O$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="305">
   <si>
     <t>TSID</t>
   </si>
@@ -904,40 +904,447 @@
     <t>Filter inventor by text</t>
   </si>
   <si>
-    <t>Fail:ClearAll button is in disable mode</t>
-  </si>
-  <si>
-    <t>Fail:MEDIUM SIZE IMAGE IS NOT DISPLAYED IN RSLARGE SIZE IMAGE IS NOT DISPLAYED IN RS</t>
-  </si>
-  <si>
-    <t>Fail:setTextSmileyTextBox is not working..org.openqa.selenium.json.JsonException: java.lang.reflect.InvocationTargetException
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-FN78GG3', ip: '192.168.0.105', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '18.0.1.1'
-Driver info: driver.version: RemoteWebDriversetTextSmileyTextBox is not working..org.openqa.selenium.json.JsonException: java.lang.reflect.InvocationTargetException
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-FN78GG3', ip: '192.168.0.105', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '18.0.1.1'
-Driver info: driver.version: RemoteWebDriver</t>
-  </si>
-  <si>
-    <t>Fail:timeout: Timed out receiving message from renderer: 300.000
-  (Session info: headless chrome=103.0.5060.114)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-FN78GG3', ip: '192.168.0.105', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '18.0.1.1'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 103.0.5060.114, chrome: {chromedriverVersion: 103.0.5060.53 (a1711811edd7..., userDataDir: C:\Users\U6070295\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:63116}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: e952f1240a31e35a494398860c14c5fc</t>
-  </si>
-  <si>
-    <t>Fail:timeout: Timed out receiving message from renderer: 300.000
-  (Session info: headless chrome=103.0.5060.114)
-Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
-System info: host: 'CLVITN-FN78GG3', ip: '192.168.0.105', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '18.0.1.1'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 103.0.5060.114, chrome: {chromedriverVersion: 103.0.5060.53 (a1711811edd7..., userDataDir: C:\Users\U6070295\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:65369}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
-Session ID: 6ea14ddfdfa3f8d111c4916d483dd29b</t>
-  </si>
-  <si>
     <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50</t>
+  </si>
+  <si>
+    <t>Fail:clickOn arrow next page is not workingjava.lang.ArrayIndexOutOfBoundsException: Index 1 out of bounds for length 1clickOn arrow next page is not workingjava.lang.ArrayIndexOutOfBoundsException: Index 1 out of bounds for length 1</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50370}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 80119777d5e70a66d5addb9fdd27c52c
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50370}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 80119777d5e70a66d5addb9fdd27c52c
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50513}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: bd323cc786d922bf37527c5c15ee1ef7
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50513}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: bd323cc786d922bf37527c5c15ee1ef7
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50552}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 776c649fbf883a2b95496c2dae5ccc89
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50552}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 776c649fbf883a2b95496c2dae5ccc89
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section.result-count &gt; div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@771bf5be (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50552}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 776c649fbf883a2b95496c2dae5ccc89waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section.result-count &gt; div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@771bf5be (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50552}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 776c649fbf883a2b95496c2dae5ccc89</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50605}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: eed22139d62fc8690124be8839fbe95d
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50605}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: eed22139d62fc8690124be8839fbe95d
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50832}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: c322e821464b224f712b69fa69a25363
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50832}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: c322e821464b224f712b69fa69a25363
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50880}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: ee342e5d2f896494496694e0389b575e
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50880}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: ee342e5d2f896494496694e0389b575e
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50982}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a1d19cbcb34e7feadaf839307cb56d35
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:50982}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: a1d19cbcb34e7feadaf839307cb56d35
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}</t>
+  </si>
+  <si>
+    <t>Fail:clickOnPYChartExpandCollapseIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;span class="mat-expansion-indicator ng-tns-c144-140 ng-trigger ng-trigger-indicatorRotate ng-star-inserted" style="transform: rotate(180deg);"&gt;&lt;/span&gt; is not clickable at point (1900, 300). Other element would receive the click: &lt;svg width="360" height="160"&gt;...&lt;/svg&gt;
+  (Session info: headless chrome=105.0.5195.102)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51099}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 09356784ebdc56212189374718ba0436clickOnPYChartExpandCollapseIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;span class="mat-expansion-indicator ng-tns-c144-140 ng-trigger ng-trigger-indicatorRotate ng-star-inserted" style="transform: rotate(180deg);"&gt;&lt;/span&gt; is not clickable at point (1900, 300). Other element would receive the click: &lt;svg width="360" height="160"&gt;...&lt;/svg&gt;
+  (Session info: headless chrome=105.0.5195.102)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51099}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 09356784ebdc56212189374718ba0436</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51141}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 8d101861de5ca095e501e8dbd93288e8
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51141}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 8d101861de5ca095e501e8dbd93288e8
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}EXPECTED AND ACTUAL PUBLICATION YEAR CHART LABEL NAMES ARE NOT MATCHINGclickOnPYChartExpandCollapseIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;span class="mat-expansion-indicator ng-tns-c144-140 ng-trigger ng-trigger-indicatorRotate ng-star-inserted" style="transform: rotate(180deg);"&gt;&lt;/span&gt; is not clickable at point (1900, 300). Other element would receive the click: &lt;svg width="360" height="160"&gt;...&lt;/svg&gt;
+  (Session info: headless chrome=105.0.5195.102)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51141}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 8d101861de5ca095e501e8dbd93288e8clickOnPYChartExpandCollapseIcon is not workingorg.openqa.selenium.ElementClickInterceptedException: element click intercepted: Element &lt;span class="mat-expansion-indicator ng-tns-c144-140 ng-trigger ng-trigger-indicatorRotate ng-star-inserted" style="transform: rotate(180deg);"&gt;&lt;/span&gt; is not clickable at point (1900, 300). Other element would receive the click: &lt;svg width="360" height="160"&gt;...&lt;/svg&gt;
+  (Session info: headless chrome=105.0.5195.102)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51141}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 8d101861de5ca095e501e8dbd93288e8</t>
+  </si>
+  <si>
+    <t>Fail:selectManageFieldCheckBoxes is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//span[@class='mat-checkbox-label'][contains(text(),'Title')]//preceding-sibling::div//input[@type='checkbox']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51381}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: e9aa76b79402524867cb30fe78878564
+*** Element info: {Using=xpath, value=//span[@class='mat-checkbox-label'][contains(text(),'Title')]//preceding-sibling::div//input[@type='checkbox']}selectManageFieldCheckBoxes is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//span[@class='mat-checkbox-label'][contains(text(),'Title')]//preceding-sibling::div//input[@type='checkbox']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51381}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: e9aa76b79402524867cb30fe78878564
+*** Element info: {Using=xpath, value=//span[@class='mat-checkbox-label'][contains(text(),'Title')]//preceding-sibling::div//input[@type='checkbox']}</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51432}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 79ccef31ad7fe79d51f15495020a7b2c
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51432}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 79ccef31ad7fe79d51f15495020a7b2c
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnLinkMoreLikeThis is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //*/section[2]//div/section/section/section[2]/section/app-result-set[1]//section[2]/div/button' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1348baad (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51432}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 79ccef31ad7fe79d51f15495020a7b2cclickOnLinkMoreLikeThis is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //*/section[2]//div/section/section/section[2]/section/app-result-set[1]//section[2]/div/button' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1348baad (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51432}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 79ccef31ad7fe79d51f15495020a7b2c</t>
+  </si>
+  <si>
+    <t>Fail:clickOnLinkSavedRecords is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: button.cdx-but-md.cdx-but-link.mat-button.mat-button-base.mat-primary &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1e60262d (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51606}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 08adf9b06aa7ceeb621517505b7b5120clickOnLinkSavedRecords is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: button.cdx-but-md.cdx-but-link.mat-button.mat-button-base.mat-primary &gt; span' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1e60262d (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51606}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 08adf9b06aa7ceeb621517505b7b5120</t>
+  </si>
+  <si>
+    <t>Fail:clickOnChemExpHomePage is not working no such element: Unable to locate element: {"method":"xpath","selector":"//a[@class='company-name']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51665}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 0359895063e1cd5574cbd629ca195f1d
+*** Element info: {Using=xpath, value=//a[@class='company-name']}clickOnChemExpHomePage is not working no such element: Unable to locate element: {"method":"xpath","selector":"//a[@class='company-name']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51665}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 0359895063e1cd5574cbd629ca195f1d
+*** Element info: {Using=xpath, value=//a[@class='company-name']}setTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@data-placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@25c89f52 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51665}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 0359895063e1cd5574cbd629ca195f1dsetTextSearchTextBox is not working..java.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //textarea[@data-placeholder='Enter keywords, phrases or text blocks to search...']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@25c89f52 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51665}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 0359895063e1cd5574cbd629ca195f1d</t>
+  </si>
+  <si>
+    <t>Fail:clickOnRSFooterGlobalCheckBox is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //app-result-paginator-bar/section/section[1]/span[1]/mat-checkbox/label/div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@6d7ba177 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51950}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: fd9ae4861283860298f66edd8e4d9f72clickOnRSFooterGlobalCheckBox is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //app-result-paginator-bar/section/section[1]/span[1]/mat-checkbox/label/div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@6d7ba177 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:51950}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: fd9ae4861283860298f66edd8e4d9f72</t>
+  </si>
+  <si>
+    <t>Fail:clickOnRSFooterGlobalCheckBox is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //app-result-paginator-bar/section/section[1]/span[1]/mat-checkbox/label/div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@75338529 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52033}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 10b85311e8654598a13c5b3f96629df7clickOnRSFooterGlobalCheckBox is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //app-result-paginator-bar/section/section[1]/span[1]/mat-checkbox/label/div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@75338529 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52033}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 10b85311e8654598a13c5b3f96629df7</t>
+  </si>
+  <si>
+    <t>Fail:isDisabledLiteratureTab is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@title='Structure search not yet available for Literature']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@6a8b24c3 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52150}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 245d3ea5a9ee6aff4c78f2904ccbc0ffisDisabledLiteratureTab is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@title='Structure search not yet available for Literature']' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@6a8b24c3 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52150}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 245d3ea5a9ee6aff4c78f2904ccbc0ff</t>
+  </si>
+  <si>
+    <t>Fail:clickOnSingleStructure is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@class='mat-card-header-text']//mat-checkbox//label//div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@17f6f008 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52377}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: e1df13b4d6c27405835756af2f45d334clickOnSingleStructure is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@class='mat-card-header-text']//mat-checkbox//label//div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@17f6f008 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52377}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: e1df13b4d6c27405835756af2f45d334</t>
+  </si>
+  <si>
+    <t>Fail:clickOnSingleStructure is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@class='mat-card-header-text']//mat-checkbox//label//div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1de8a37 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52602}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: cc3ff2acc3871611498cc447ccb748c1clickOnSingleStructure is not workingjava.lang.Exception: waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //div[@class='mat-card-header-text']//mat-checkbox//label//div/input' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@1de8a37 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52602}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: cc3ff2acc3871611498cc447ccb748c1</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52714}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 51505d227be6e01fd6b7cc1e03a240fe
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52714}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 51505d227be6e01fd6b7cc1e03a240fe
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //h4[contains(.,'Edit existing cluster items')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@54a48703 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52714}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 51505d227be6e01fd6b7cc1e03a240fewaitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.xpath: //h4[contains(.,'Edit existing cluster items')]' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@54a48703 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52714}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 51505d227be6e01fd6b7cc1e03a240fe</t>
+  </si>
+  <si>
+    <t>Fail:clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52777}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 53ca6f19ce1c9a54cb5b9a3c2c30bdaf
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52777}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 53ca6f19ce1c9a54cb5b9a3c2c30bdaf
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52777}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 53ca6f19ce1c9a54cb5b9a3c2c30bdaf
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}clickOnTabLiterature is not workingno such element: Unable to locate element: {"method":"xpath","selector":"//*[@id='tab-2']"}
+  (Session info: headless chrome=105.0.5195.102)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:52777}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 53ca6f19ce1c9a54cb5b9a3c2c30bdaf
+*** Element info: {Using=xpath, value=//*[@id='tab-2']}</t>
+  </si>
+  <si>
+    <t>Fail:waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section.result-count &gt; div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@29e52142 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53493}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: e1024d7bba6d2ff67f077aded51ed04bwaitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section.result-count &gt; div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@29e52142 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.102, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53493}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: e1024d7bba6d2ff67f077aded51ed04b</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Fail:waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section.result-count &gt; div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@665224b4 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.127, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57875}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: faad4a59a4ae9c859bd1b3d80e33ae32waitUntilElementIsDisplayed is not working.. :: Proxy element for: DefaultElementLocator 'By.cssSelector: section.result-count &gt; div' org.openqa.selenium.TimeoutException: Expected condition failed: waiting for support.Controller$1@665224b4 (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'BLR-5NJH5Y2-10L', ip: '192.168.1.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '11.0.7'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 105.0.5195.127, chrome: {chromedriverVersion: 105.0.5195.52 (412c95e51883..., userDataDir: C:\Users\U6052550\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:57875}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: faad4a59a4ae9c859bd1b3d80e33ae32</t>
   </si>
 </sst>
 </file>
@@ -945,9 +1352,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -983,6 +1390,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1034,14 +1448,14 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1050,6 +1464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="6" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1401,14 +1816,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.109375" style="1" collapsed="1"/>
+    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1419,7 +1834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1437,34 +1852,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}">
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="69.33203125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="69.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="23" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="56.77734375" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="4.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="255" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.33203125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.33203125" style="5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="70.44140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="40" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="203.33203125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="132.109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.88671875" style="5" collapsed="1"/>
-    <col min="15" max="15" width="28" style="5" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="27.44140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="16384" width="8.88671875" style="5" collapsed="1"/>
+    <col min="4" max="4" width="56.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="255" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="39.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="70.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="40" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="203.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="132.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8.85546875" style="5" collapsed="1"/>
+    <col min="14" max="14" width="28" style="5" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="27.42578125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.85546875" style="5" collapsed="1"/>
+    <col min="17" max="17" width="8.85546875" style="5"/>
+    <col min="18" max="16384" width="8.85546875" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1480,39 +1896,38 @@
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="G1" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>80</v>
+        <v>191</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="P1" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>81</v>
       </c>
@@ -1528,20 +1943,20 @@
       <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G2" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>82</v>
       </c>
@@ -1557,20 +1972,20 @@
       <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F3" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G3" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>83</v>
       </c>
@@ -1586,20 +2001,20 @@
       <c r="E4" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F4" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G4" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J4" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>84</v>
       </c>
@@ -1615,20 +2030,20 @@
       <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F5" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G5" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J5" s="6" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>85</v>
       </c>
@@ -1644,20 +2059,20 @@
       <c r="E6" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F6" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G6" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>86</v>
       </c>
@@ -1673,23 +2088,23 @@
       <c r="E7" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F7" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G7" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>263</v>
+        <v>31</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>87</v>
       </c>
@@ -1705,23 +2120,23 @@
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F8" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G8" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>263</v>
+        <v>35</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>88</v>
       </c>
@@ -1737,23 +2152,23 @@
       <c r="E9" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F9" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G9" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>263</v>
+        <v>35</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>89</v>
       </c>
@@ -1769,20 +2184,20 @@
       <c r="E10" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F10" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G10" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J10" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>90</v>
       </c>
@@ -1798,23 +2213,23 @@
       <c r="E11" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F11" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G11" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>263</v>
+        <v>20</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>91</v>
       </c>
@@ -1830,23 +2245,23 @@
       <c r="E12" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F12" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G12" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>263</v>
+        <v>20</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>93</v>
       </c>
@@ -1862,23 +2277,23 @@
       <c r="E13" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F13" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G13" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>263</v>
+        <v>20</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>94</v>
       </c>
@@ -1894,23 +2309,23 @@
       <c r="E14" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F14" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G14" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>263</v>
+        <v>20</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>95</v>
       </c>
@@ -1926,23 +2341,23 @@
       <c r="E15" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F15" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G15" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>263</v>
+        <v>35</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>96</v>
       </c>
@@ -1958,20 +2373,20 @@
       <c r="E16" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F16" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G16" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J16" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>97</v>
       </c>
@@ -1987,20 +2402,20 @@
       <c r="E17" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F17" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G17" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J17" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>98</v>
       </c>
@@ -2016,20 +2431,20 @@
       <c r="E18" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F18" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G18" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J18" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>99</v>
       </c>
@@ -2045,20 +2460,20 @@
       <c r="E19" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F19" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G19" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J19" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -2074,20 +2489,20 @@
       <c r="E20" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F20" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G20" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J20" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>101</v>
       </c>
@@ -2103,26 +2518,26 @@
       <c r="E21" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F21" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G21" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J21" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="K21" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="L21" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M21" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>104</v>
       </c>
@@ -2138,20 +2553,20 @@
       <c r="E22" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F22" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G22" s="6" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J22" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>106</v>
       </c>
@@ -2167,20 +2582,20 @@
       <c r="E23" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F23" s="6" t="s">
+        <v>281</v>
+      </c>
       <c r="G23" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J23" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>107</v>
       </c>
@@ -2196,17 +2611,17 @@
       <c r="E24" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F24" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G24" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>108</v>
       </c>
@@ -2222,20 +2637,20 @@
       <c r="E25" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F25" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G25" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J25" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>109</v>
       </c>
@@ -2251,20 +2666,20 @@
       <c r="E26" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F26" s="6" t="s">
+        <v>304</v>
+      </c>
       <c r="G26" s="6" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J26" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>110</v>
       </c>
@@ -2280,23 +2695,23 @@
       <c r="E27" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F27" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G27" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J27" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="L27" s="6" t="s">
+      <c r="K27" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>112</v>
       </c>
@@ -2312,20 +2727,20 @@
       <c r="E28" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F28" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G28" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J28" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>115</v>
       </c>
@@ -2341,20 +2756,20 @@
       <c r="E29" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F29" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G29" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J29" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>118</v>
       </c>
@@ -2370,20 +2785,20 @@
       <c r="E30" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F30" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G30" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J30" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>121</v>
       </c>
@@ -2399,20 +2814,20 @@
       <c r="E31" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="F31" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G31" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J31" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>124</v>
       </c>
@@ -2428,136 +2843,136 @@
       <c r="E32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>262</v>
+      <c r="F32" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J32" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="6" t="s">
+      <c r="C33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>262</v>
+      <c r="E33" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J33" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="6" t="s">
+      <c r="C34" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>262</v>
+      <c r="E34" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J34" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="C35" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>262</v>
+      <c r="E35" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J35" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="6" t="s">
+      <c r="C36" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>262</v>
+      <c r="E36" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J36" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>136</v>
       </c>
@@ -2573,20 +2988,20 @@
       <c r="E37" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>262</v>
+      <c r="F37" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J37" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>139</v>
       </c>
@@ -2602,78 +3017,78 @@
       <c r="E38" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>262</v>
+      <c r="F38" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J38" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="C39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>262</v>
+      <c r="E39" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J39" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="6" t="s">
+      <c r="C40" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>262</v>
+      <c r="E40" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J40" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>148</v>
       </c>
@@ -2689,49 +3104,49 @@
       <c r="E41" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>262</v>
+      <c r="F41" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J41" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="6" t="s">
+      <c r="C42" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>3</v>
+      <c r="E42" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>288</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J42" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>166</v>
       </c>
@@ -2747,20 +3162,20 @@
       <c r="E43" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>262</v>
+      <c r="F43" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J43" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>167</v>
       </c>
@@ -2776,49 +3191,49 @@
       <c r="E44" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>262</v>
+      <c r="F44" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J44" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
+    <row r="45" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="6" t="s">
+      <c r="C45" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E45" s="6" t="s">
-        <v>3</v>
+      <c r="E45" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>290</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J45" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>169</v>
       </c>
@@ -2834,20 +3249,20 @@
       <c r="E46" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>262</v>
+      <c r="F46" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J46" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>170</v>
       </c>
@@ -2863,20 +3278,20 @@
       <c r="E47" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>262</v>
+      <c r="F47" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J47" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>171</v>
       </c>
@@ -2892,20 +3307,20 @@
       <c r="E48" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>262</v>
+      <c r="F48" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J48" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>187</v>
       </c>
@@ -2921,49 +3336,49 @@
       <c r="E49" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G49" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>262</v>
+      <c r="F49" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J49" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
+    <row r="50" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="6" t="s">
+      <c r="C50" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="E50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H50" s="7" t="s">
-        <v>262</v>
+      <c r="E50" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J50" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>189</v>
       </c>
@@ -2979,20 +3394,20 @@
       <c r="E51" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G51" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>262</v>
+      <c r="F51" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J51" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>190</v>
       </c>
@@ -3008,20 +3423,20 @@
       <c r="E52" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G52" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>262</v>
+      <c r="F52" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J52" s="6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>206</v>
       </c>
@@ -3037,20 +3452,20 @@
       <c r="E53" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G53" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H53" s="7" t="s">
-        <v>262</v>
+      <c r="F53" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J53" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>207</v>
       </c>
@@ -3066,20 +3481,20 @@
       <c r="E54" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G54" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>262</v>
+      <c r="F54" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J54" s="6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>202</v>
       </c>
@@ -3095,20 +3510,20 @@
       <c r="E55" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G55" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>262</v>
+      <c r="F55" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J55" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>203</v>
       </c>
@@ -3124,20 +3539,20 @@
       <c r="E56" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G56" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>262</v>
+      <c r="F56" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J56" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>204</v>
       </c>
@@ -3153,20 +3568,20 @@
       <c r="E57" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G57" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>262</v>
+      <c r="F57" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J57" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>211</v>
       </c>
@@ -3182,20 +3597,20 @@
       <c r="E58" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G58" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H58" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="I58" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="O58" s="6" t="s">
+      <c r="F58" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="N58" s="6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>215</v>
       </c>
@@ -3211,26 +3626,26 @@
       <c r="E59" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G59" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H59" s="7" t="s">
-        <v>262</v>
+      <c r="F59" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>263</v>
+        <v>20</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K59" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="O59" s="6" t="s">
+      <c r="N59" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>220</v>
       </c>
@@ -3246,23 +3661,23 @@
       <c r="E60" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G60" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>262</v>
+      <c r="F60" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J60" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="O60" s="6" t="s">
+      <c r="N60" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>234</v>
       </c>
@@ -3278,26 +3693,26 @@
       <c r="E61" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G61" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>262</v>
+      <c r="F61" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>263</v>
+        <v>20</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K61" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="O61" s="6" t="s">
+      <c r="N61" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>235</v>
       </c>
@@ -3313,23 +3728,23 @@
       <c r="E62" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H62" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="I62" s="6" t="s">
-        <v>263</v>
+      <c r="F62" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="N62" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="O62" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="P62" s="6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>236</v>
       </c>
@@ -3345,23 +3760,23 @@
       <c r="E63" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G63" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="H63" s="7" t="s">
-        <v>262</v>
+      <c r="F63" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J63" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="O63" s="6" t="s">
+      <c r="N63" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>237</v>
       </c>
@@ -3377,26 +3792,26 @@
       <c r="E64" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G64" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H64" s="7" t="s">
-        <v>262</v>
+      <c r="F64" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>263</v>
+        <v>20</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K64" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="O64" s="6" t="s">
+      <c r="N64" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>241</v>
       </c>
@@ -3412,49 +3827,49 @@
       <c r="E65" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G65" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>262</v>
+      <c r="F65" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J65" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
+    <row r="66" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="C66" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D66" s="6" t="s">
+      <c r="C66" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="E66" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>262</v>
+      <c r="E66" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J66" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>247</v>
       </c>
@@ -3470,20 +3885,20 @@
       <c r="E67" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G67" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H67" s="7" t="s">
-        <v>262</v>
+      <c r="F67" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J67" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>250</v>
       </c>
@@ -3499,23 +3914,23 @@
       <c r="E68" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G68" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>262</v>
+      <c r="F68" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J68" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O68" s="6" t="s">
+      <c r="N68" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>240</v>
       </c>
@@ -3531,23 +3946,23 @@
       <c r="E69" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G69" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H69" s="7" t="s">
-        <v>262</v>
+      <c r="F69" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>263</v>
+        <v>114</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="K69" s="6" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>258</v>
       </c>
@@ -3563,20 +3978,20 @@
       <c r="E70" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G70" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H70" s="7" t="s">
-        <v>262</v>
+      <c r="F70" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J70" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>257</v>
       </c>
@@ -3592,20 +4007,20 @@
       <c r="E71" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G71" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H71" s="7" t="s">
-        <v>262</v>
+      <c r="F71" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J71" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>261</v>
       </c>
@@ -3624,20 +4039,17 @@
       <c r="F72" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="G72" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H72" s="7" t="s">
-        <v>262</v>
+      <c r="G72" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J72" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>275</v>
       </c>
@@ -3653,20 +4065,20 @@
       <c r="E73" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G73" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="H73" s="7" t="s">
-        <v>262</v>
+      <c r="F73" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J73" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>276</v>
       </c>
@@ -3682,20 +4094,20 @@
       <c r="E74" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G74" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H74" s="7" t="s">
-        <v>262</v>
+      <c r="F74" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J74" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>277</v>
       </c>
@@ -3711,20 +4123,20 @@
       <c r="E75" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G75" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H75" s="7" t="s">
-        <v>262</v>
+      <c r="F75" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J75" s="6" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>278</v>
       </c>
@@ -3740,35 +4152,35 @@
       <c r="E76" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G76" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>262</v>
+      <c r="F76" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="K76" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="O76" s="6" t="s">
+      <c r="N76" s="6" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K78" s="6"/>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J78" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P76" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}"/>
+  <autoFilter ref="A1:O76" xr:uid="{AF3C60A3-C1CE-454B-9E25-9FD950A53520}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H32" r:id="rId1" xr:uid="{6F89064E-1AF0-40D6-9F7A-013C19036A8D}"/>
-    <hyperlink ref="H33" r:id="rId2" xr:uid="{6D5316C2-75A8-43D3-8673-975B13E163F3}"/>
-    <hyperlink ref="H34:H36" r:id="rId3" display="anand.perumallukamichetty@clarivate.com" xr:uid="{26AAD26D-35D4-4232-8D22-B391C245DF53}"/>
+    <hyperlink ref="G32" r:id="rId1" xr:uid="{6F89064E-1AF0-40D6-9F7A-013C19036A8D}"/>
+    <hyperlink ref="G33" r:id="rId2" xr:uid="{6D5316C2-75A8-43D3-8673-975B13E163F3}"/>
+    <hyperlink ref="G34:G36" r:id="rId3" display="anand.perumallukamichetty@clarivate.com" xr:uid="{26AAD26D-35D4-4232-8D22-B391C245DF53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>

</xml_diff>

<commit_message>
Test case ID updated for Literature Citation & ViewAsResultSet
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AF6F5B-3E63-4A1A-8FB5-A61CB1BC6B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24801D04-0A8F-4A39-A39C-C227ED270D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="289">
   <si>
     <t>TSID</t>
   </si>
@@ -904,15 +904,6 @@
     <t>validateLiteratureCitations</t>
   </si>
   <si>
-    <t>Literature citations</t>
-  </si>
-  <si>
-    <t>CHEMEXP-2001</t>
-  </si>
-  <si>
-    <t>CHEMEXP-2002</t>
-  </si>
-  <si>
     <t>validate - view as results set for Literature - Citing Literature and Cited Literature</t>
   </si>
   <si>
@@ -926,6 +917,34 @@
   </si>
   <si>
     <t>Derwent@2022</t>
+  </si>
+  <si>
+    <t>Literature citations.</t>
+  </si>
+  <si>
+    <t>CHEMEXP-2167</t>
+  </si>
+  <si>
+    <t>CHEMEXP-2168</t>
+  </si>
+  <si>
+    <t>Fail:deSelectMultiplePublicationChartFilters is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"css selector","selector":"#publ_year_rect_2010"}
+  (Session info: headless chrome=106.0.5249.119)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-FN78GG3', ip: '192.168.0.100', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '18.0.1.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 106.0.5249.119, chrome: {chromedriverVersion: 106.0.5249.61 (511755355844..., userDataDir: C:\Users\U6070295\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53921}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 09b26f7de90ac8b0780d926519b09660
+*** Element info: {Using=css selector, value=#publ_year_rect_2010}deSelectMultiplePublicationChartFilters is not working..org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"css selector","selector":"#publ_year_rect_2010"}
+  (Session info: headless chrome=106.0.5249.119)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'CLVITN-FN78GG3', ip: '192.168.0.100', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '18.0.1.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 106.0.5249.119, chrome: {chromedriverVersion: 106.0.5249.61 (511755355844..., userDataDir: C:\Users\U6070295\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:53921}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 09b26f7de90ac8b0780d926519b09660
+*** Element info: {Using=css selector, value=#publ_year_rect_2010}</t>
   </si>
 </sst>
 </file>
@@ -1425,7 +1444,7 @@
   <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,10 +1534,10 @@
         <v>175</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>20</v>
@@ -1544,10 +1563,10 @@
         <v>175</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>17</v>
@@ -1573,10 +1592,10 @@
         <v>175</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>23</v>
@@ -1602,10 +1621,10 @@
         <v>175</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>205</v>
@@ -1631,10 +1650,10 @@
         <v>175</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>23</v>
@@ -1660,10 +1679,10 @@
         <v>175</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>31</v>
@@ -1692,10 +1711,10 @@
         <v>175</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>35</v>
@@ -1724,10 +1743,10 @@
         <v>175</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>35</v>
@@ -1756,10 +1775,10 @@
         <v>175</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>20</v>
@@ -1785,10 +1804,10 @@
         <v>175</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>20</v>
@@ -1817,10 +1836,10 @@
         <v>175</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>20</v>
@@ -1849,10 +1868,10 @@
         <v>175</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>20</v>
@@ -1881,10 +1900,10 @@
         <v>175</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>20</v>
@@ -1913,10 +1932,10 @@
         <v>175</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>35</v>
@@ -1945,16 +1964,16 @@
         <v>175</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>209</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1977,10 +1996,10 @@
         <v>175</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>17</v>
@@ -2006,10 +2025,10 @@
         <v>175</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>67</v>
@@ -2035,10 +2054,10 @@
         <v>175</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>17</v>
@@ -2064,10 +2083,10 @@
         <v>175</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>23</v>
@@ -2093,10 +2112,10 @@
         <v>175</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>20</v>
@@ -2128,10 +2147,10 @@
         <v>175</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>114</v>
@@ -2157,10 +2176,10 @@
         <v>175</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>23</v>
@@ -2186,10 +2205,10 @@
         <v>175</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2212,10 +2231,10 @@
         <v>175</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>23</v>
@@ -2241,10 +2260,10 @@
         <v>175</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>23</v>
@@ -2270,10 +2289,10 @@
         <v>175</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>72</v>
@@ -2302,10 +2321,10 @@
         <v>175</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>114</v>
@@ -2331,10 +2350,10 @@
         <v>175</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>105</v>
@@ -2360,10 +2379,10 @@
         <v>175</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>105</v>
@@ -2389,10 +2408,10 @@
         <v>175</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>105</v>
@@ -2418,10 +2437,10 @@
         <v>175</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>105</v>
@@ -2447,10 +2466,10 @@
         <v>175</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>105</v>
@@ -2476,10 +2495,10 @@
         <v>175</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>105</v>
@@ -2505,10 +2524,10 @@
         <v>175</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>105</v>
@@ -2534,10 +2553,10 @@
         <v>175</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I36" s="6" t="s">
         <v>105</v>
@@ -2563,10 +2582,10 @@
         <v>175</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>114</v>
@@ -2592,10 +2611,10 @@
         <v>175</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>114</v>
@@ -2621,10 +2640,10 @@
         <v>175</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>114</v>
@@ -2650,10 +2669,10 @@
         <v>175</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>114</v>
@@ -2679,10 +2698,10 @@
         <v>175</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>114</v>
@@ -2708,10 +2727,10 @@
         <v>175</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I42" s="6" t="s">
         <v>114</v>
@@ -2737,10 +2756,10 @@
         <v>175</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I43" s="6" t="s">
         <v>156</v>
@@ -2763,13 +2782,13 @@
         <v>3</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>175</v>
+        <v>288</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>20</v>
@@ -2795,10 +2814,10 @@
         <v>175</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>20</v>
@@ -2824,10 +2843,10 @@
         <v>175</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>162</v>
@@ -2853,10 +2872,10 @@
         <v>175</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>164</v>
@@ -2882,10 +2901,10 @@
         <v>175</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I48" s="6" t="s">
         <v>23</v>
@@ -2911,10 +2930,10 @@
         <v>175</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>179</v>
@@ -2940,10 +2959,10 @@
         <v>175</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>20</v>
@@ -2969,10 +2988,10 @@
         <v>175</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>102</v>
@@ -2998,10 +3017,10 @@
         <v>175</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>186</v>
@@ -3027,10 +3046,10 @@
         <v>175</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>102</v>
@@ -3056,10 +3075,10 @@
         <v>175</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I54" s="6" t="s">
         <v>186</v>
@@ -3085,10 +3104,10 @@
         <v>175</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I55" s="6" t="s">
         <v>20</v>
@@ -3114,10 +3133,10 @@
         <v>175</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I56" s="6" t="s">
         <v>20</v>
@@ -3143,10 +3162,10 @@
         <v>175</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I57" s="6" t="s">
         <v>23</v>
@@ -3172,10 +3191,10 @@
         <v>175</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N58" s="6" t="s">
         <v>214</v>
@@ -3201,10 +3220,10 @@
         <v>175</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I59" s="6" t="s">
         <v>20</v>
@@ -3236,10 +3255,10 @@
         <v>175</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I60" s="6" t="s">
         <v>223</v>
@@ -3268,10 +3287,10 @@
         <v>175</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I61" s="6" t="s">
         <v>20</v>
@@ -3303,10 +3322,10 @@
         <v>175</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N62" s="6" t="s">
         <v>219</v>
@@ -3335,10 +3354,10 @@
         <v>175</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I63" s="6" t="s">
         <v>20</v>
@@ -3367,10 +3386,10 @@
         <v>175</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I64" s="6" t="s">
         <v>20</v>
@@ -3402,10 +3421,10 @@
         <v>175</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I65" s="6" t="s">
         <v>20</v>
@@ -3431,10 +3450,10 @@
         <v>175</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I66" s="6" t="s">
         <v>23</v>
@@ -3460,10 +3479,10 @@
         <v>175</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>20</v>
@@ -3489,10 +3508,10 @@
         <v>175</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I68" s="6" t="s">
         <v>23</v>
@@ -3521,10 +3540,10 @@
         <v>175</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I69" s="6" t="s">
         <v>114</v>
@@ -3553,10 +3572,10 @@
         <v>175</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I70" s="6" t="s">
         <v>20</v>
@@ -3582,10 +3601,10 @@
         <v>175</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I71" s="6" t="s">
         <v>20</v>
@@ -3611,10 +3630,10 @@
         <v>175</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I72" s="6" t="s">
         <v>20</v>
@@ -3640,10 +3659,10 @@
         <v>175</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I73" s="6" t="s">
         <v>23</v>
@@ -3669,10 +3688,10 @@
         <v>175</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I74" s="6" t="s">
         <v>20</v>
@@ -3698,10 +3717,10 @@
         <v>175</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I75" s="6" t="s">
         <v>271</v>
@@ -3727,10 +3746,10 @@
         <v>175</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I76" s="6" t="s">
         <v>270</v>
@@ -3744,10 +3763,10 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>14</v>
@@ -3762,10 +3781,10 @@
         <v>175</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I77" s="6" t="s">
         <v>23</v>
@@ -3773,16 +3792,16 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>3</v>
@@ -3791,10 +3810,10 @@
         <v>175</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>186</v>

</xml_diff>